<commit_message>
Add some pubs from Chris Connell
</commit_message>
<xml_diff>
--- a/test-science-documents-library.xlsx
+++ b/test-science-documents-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhaman\Documents\test-science-documents-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AACBAF-7617-4186-9FBB-69CEF1A179E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1BF12-B7D4-4E27-B7E7-B5E598551F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12337" yWindow="5925" windowWidth="21599" windowHeight="11528" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
+    <workbookView xWindow="-98" yWindow="353" windowWidth="28996" windowHeight="15944" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="862">
   <si>
     <t>Project</t>
   </si>
@@ -3992,13 +3992,489 @@
       </rPr>
       <t>. IDA Product ID 3002009. Alexandria, VA: Institute for Defense Analyses, 2024.</t>
     </r>
+  </si>
+  <si>
+    <t>Continuous Metrics for Efficient and Effective Testing</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=c38f1184-1ea8-48ac-81fe-d76f56b4149b</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	In today’s fiscal environment, efficient and effective testing is essential. Often, military system requirements are defined using probability of success as the primary measure of effectiveness – for example, a system must complete its mission 80 percent of the time; or the system must detect 90 percent of targets. The traditional approach to testing these probability-based requirements is to execute a series of trials and then total the number of successes; the ratio of successes to number of trails provides an intuitive measure of the probability of success. However, this method of testing has proven to be cost prohibitive, especially at high levels of statistical confidence and power. Often, one or more continuous metrics empirically related to the probability based metric provide more information about system performance than the pass/fail construct. Using these metrics in lieu of the probability-based metrics to plan testing both reduces test costs and provides a better understanding of system performance. In this talk the authors discusses the cost of using binary test metrics (e.g., success or failure, hit or miss). They present several common T&amp;E examples, translating the original probability based requirement to a related continuous metric, and show potential cost savings and information gain achieved by the conversion.</t>
+  </si>
+  <si>
+    <t>Alyson Wilson, Robert Holcomb, Lee Dewald, Samuel Parry</t>
+  </si>
+  <si>
+    <t>A Bayesian Approach to Evaluation of Land Warfare Systems</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=f7d33615-62d5-4177-bf90-ae16701be0e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This presentation is a presentation for the Army Conference on Applied Statistics. The presentation covers a brief introduction to land warfare problems, and devises a methodology using Bayes Theorem to estimate parameters of interest. Two examples are given, a simple one using independent Bernoulli Trials, and a more complex one using correlated Red and Blue casualty data in a Loss Exchange Ratio and a hierarchical model. The presentation demonstrates that the Bayesian approach is successful in both examples at reducing the variance of the estimated parameters, potentially reducing the cost of devising a complex test program. The presentation concludes with suggested next steps applicable to the Army Ground Combat Vehicle program.</t>
+  </si>
+  <si>
+    <t>Design of Experiments (DOE) provides a rigorous methodology for developing and evaluating test plans. Design excellence consists of having enough test points placed in the right locations in the operational envelope to answer the questions of interest for the test. The key aspects of a well-designed experiment include: the goal of the test, the response variables, the factors and levels, a method for strategically varying the factors across the operational envelope, and statistical measures of merit. Currently, the majority of test plans utilize statistical measures of merit based on confidence and power. Although important, confidence and power are not the only measure of the adequacy and merit of a test design. The type of method that is appropriate is dependent on the goal of the test and the experimental design methodology used. There is no one-size-fits-all solution; rather there is a collection of useful tools that apply in various combinations for different test goals and designs. This talk outlines different statistical measures of merit that should be used when planning an operational test.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=16e6bb81-6c66-4523-bf3f-750d941f0dc9</t>
+  </si>
+  <si>
+    <t>Design of Experiments for In-Lab Operational Testing of the AN/BQQ-10 Submarine Sonar System</t>
+  </si>
+  <si>
+    <t>Laura Freeman, Justace Clutter, George Khoury</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=d739ca92-dd54-4be6-963a-697f6eff843c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operational testing of the AN/BQQ-10 submarine sonar system has never been able to show significant improvements in software versions because of the high variability of at sea measurements. To mitigate this problem, in the most recent AN/BQQ-10 operational test, the Navy’s operational test agency (in consultation with IDA under the direction of Director, Operational Test and Evaluation) supplemented the at sea testing with an operationally focused in-lab comparison. This test used recorded real data played back on two different versions of the sonar system. For each version, the test recorded the time it took multiple operations, with varying operational experience, to detect a submarine target once it appeared on the display. This new test methodology had several benefits: (1) the laboratory setting allowed for the use of design of experiments to control factors that are traditionally infeasible to control during an at sea test; (2) the direct comparison between the two systems resulted in demonstrating a statistically significant reduction in the detection time for the new system. Although laboratory testing cannot replace at sea testing, the results provide strong indication that we can expect performance improvements in the operational environment. This case study shows that laboratory testing and design of experiments have a place in operational testing and should be expanded to improve testing for other systems. </t>
+  </si>
+  <si>
+    <t>Applying Risk Analysis to Acceptance Testing of Combat Helmets</t>
+  </si>
+  <si>
+    <t>Janice Hester, Laura Freeman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acceptance testing of combat helmets presents multiple challenges that require statistically-sound solutions. For example, how should first article and lot acceptance tests treat multiple threats and measures of performance? How should these tests account for multiple helmet sizes and environmental treatments? How closely should first article testing requirements match historical or characterization test data? What government and manufacturer risks are acceptable during lot acceptance testing? Similar challenges arise when testing other components of Personal Protective Equipment and similar statistical approaches should be applied to all components. This presentation explores these questions using operating characteristics curves and simulation studies.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=1fc6a753-ed24-4122-8444-f8ff497d3db4</t>
+  </si>
+  <si>
+    <t>Surveys in Operational Test and Evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recently Dr. Gilmore, DOT&amp;E, signed out a memo providing Guidance on the Use and Design of Surveys in Operational Test and Evaluation. This guidance memo helps the Human Systems Integration (HSI) community to ensure that useful and accurate HSI data are collected. Information about how HSI experts can leverage the guidance is presented. Specifically, the presentation will cover which HSI metrics can and cannot be answered by surveys. </t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=a9377019-792c-48df-8b2f-517630e5ace7</t>
+  </si>
+  <si>
+    <t>Introduction to Survey Design</t>
+  </si>
+  <si>
+    <t>Heather Wojton, Justin Mary, Jonathan Snavely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	An important goal of test and evaluation is to understand not only how a system performs in its intended environment, but also users’ experiences operating the system. This briefing aimed to provide the audience with a set of tools – most notably, surveys – that are appropriate for measuring the user experience. DOT&amp;E guidance regarding these tools is highlighted where appropriate. The briefing was broken into three major sections: conceptualizing surveys, writing survey items, and formatting surveys. At the end of this briefing, the audience should have a better understanding of the value and purpose of surveys and how to construct them.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=96ed151f-b7fe-44db-8c04-72d5367b38cf</t>
+  </si>
+  <si>
+    <t>survey design, human factors, research methods</t>
+  </si>
+  <si>
+    <t>Tutorial on Sensitivity Testing in Live Fire Test and Evaluation</t>
+  </si>
+  <si>
+    <t>Laura Freeman, Thomas Johnson, Raymond Chen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	A sensitivity experiment is a special type of experimental design that is used when the response variable is binary and the covariate is continuous. Armor protection and projectile lethality tests often use sensitivity experiments to characterize a projectile's probability of penetrating the armor. In this mini-tutorial we illustrate the challenge of modeling a binary response with a limited sample size, and show how sensitivity experiments can mitigate this problem. We review eight different single covariate sensitivity experiments and present a comparison of these designs using simulation. Additionally, we cover sensitivity experiments for cases that include more than one covariate, and highlight recent research in this area.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=5db28187-d971-4cc8-9931-fefd5c670da5</t>
+  </si>
+  <si>
+    <t>Matthew Avery, Rebecca Medlin, Jonathan Bell, Laura Freeman</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=80253af1-f2bc-4d7c-8fd0-8f8e6e417d85</t>
+  </si>
+  <si>
+    <t>This reliability course provides information to assist DOT&amp;E action officers in their review and assessment of system reliability. Course briefings cover reliability planning and analysis activities that span the acquisition life cycle. Each briefing discusses review criteria relevant to DOT&amp;E action officers based on DoD policies and lessons learned from previous oversight efforts.</t>
+  </si>
+  <si>
+    <t>DOT&amp;E Reliability Course</t>
+  </si>
+  <si>
+    <t>Kassandra Fronczyk</t>
+  </si>
+  <si>
+    <t>Bayesian Analysis in R/STAN</t>
+  </si>
+  <si>
+    <t>Bayesian statistics, Reliability, combining information</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In an era of reduced budgets and limited testing, verifying that requirements have been met in a single test period can be challenging, particularly using traditional analysis methods that ignore all available information. The Bayesian paradigm is tailor made for these situations, allowing for the combination of multiple sources of data and resulting in more robust inference and uncertainty quantification. Consequently, Bayesian analyses are becoming increasingly popular in T&amp;E. This tutorial briefly introduces the basic concepts of Bayesian Statistics, with implementation details illustrated in R through two case studies: reliability for the Core Mission functional area of the Littoral Combat Ship (LCS) and performance curves for a chemical detector in the Bio-chemical Detection System (BDS) with different agents and matrices. Examples are also presented using STAN, a high-performance open-source software for Bayesian inference on multi-level models. </t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=44196261-645f-4a40-84ff-43074b9442fe</t>
+  </si>
+  <si>
+    <t>Science of Test Workshop Proceedings, April 11-13, 2016</t>
+  </si>
+  <si>
+    <t>Laura Freeman, Pamela Rambow, Jonathan Snavely</t>
+  </si>
+  <si>
+    <t>Leadership Perspective, Science of Test Workshop, statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	To mark IDA's 60th anniversary, we are conducting a series of workshops and symposia that bring together IDA sponsors, researchers, experts inside and outside government, and other stakeholders to discuss issues of the day. These events focus on future national security challenges, reflecting on how past lessons and accomplishments help prepare us to deal with complex issues and environments we face going forward. This publication represents the proceedings of the Science of Test Workshop. </t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=f2f6c082-e2da-4cc6-a6a7-1bbc34568f85</t>
+  </si>
+  <si>
+    <t>Daniel Porter, Emily Fedele, Heather Wojton</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=6a8b993a-1ef4-47f6-adaf-6ee915be4275</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	Pilot Training Next is an exploratory investigation of new technologies and procedures to increase the efficiency of Undergraduate Pilot Training in the United States Air Force. IDA analysts present a method of quantifying skill transfer from simulators to aircraft under realistic, uncontrolled conditions. </t>
+  </si>
+  <si>
+    <t>Introduction to Bayesian Analysis</t>
+  </si>
+  <si>
+    <t>John Haman, Keyla Pagan-Rivera, Rebecca Medlin, Heather Wojton</t>
+  </si>
+  <si>
+    <t>Bayesian, Defense Testing, Analyses</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	As operational testing becomes increasingly integrated and research questions become more difficult to answer, IDA’s Test Science team has found Bayesian models to be powerful data analysis methods. Analysts and decision-makers should understand the differences between this approach and the conventional way of analyzing data. It is also important to recognize when an analysis could benefit from the inclusion of prior information—what we already know about a system’s performance—and to understand the proper way to incorporate that information. To apply Bayesian methods, analysts need to comprehend some technical aspects of this approach and know how to properly use appropriate statistical software. In this course, students learn the intuition behind Bayesian statistics, the mathematical details of posterior distributions, how to fit simple Bayesian models using computer software, and how to assess model fit.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=5e495bf2-f42a-4dc9-b284-090142de5a0d</t>
+  </si>
+  <si>
+    <t>Thoughts on Applying Design of Experiments (DOE) to Cyber Testing</t>
+  </si>
+  <si>
+    <t>Michael Gilmore, Rebecca Medlin, Kelly Avery, Matthew Girardi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This briefing presented at Dataworks 2022 provides examples of potential ways in which Design of Experiments (DOE) could be applied to initially scope cyber assessments and, based on the results of those assessments, subsequently design in greater detail cyber tests.</t>
+  </si>
+  <si>
+    <t>https://libweb.ida.org/sydneyplus/sydneyplus/ViewRecord.aspx?template=Publicatio&amp;record=61338bca-90be-45b4-ab0e-1513c1882b3f</t>
+  </si>
+  <si>
+    <t>Freeman, Laura J, and V Bram Lillard. Continuous Metrics for Efficient and Effective Testing. IDA Document NS D-4571. Alexandria, VA: Institute for Defense Analyses, 2012.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wilson, Alyson, Lee Dewald, Robert Holcomb, and Samuel Parry. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A Bayesian Approach to Evaluation  of Land Warfare Systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-4711. Alexandria, VA: Institute for Defense Analyses, 2012.</t>
+    </r>
+  </si>
+  <si>
+    <t>Freeman, Laura. Scientific Test and Analysis Techniques: Statistical Measures of Merit. IDA Document D-5070. Alexandria, VA: Institute for Defense Analyses, 2014.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clutter, Justace R, George Khoury, and Laura Freeman. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Design of Experiments for In-Lab Operational Testing of the AN/BQQ-10 Submarine Sonar System</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-5486. Alexandria, VA: Institute for Defense Analyses, 2014.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hester, Janice, and Laura Freeman. Applying Risk Analysis to Acceptance Testing of Combat Helmets. IDA Document NS D-5334. Alexandria, VA: Institute for Defense Analyses, 2014.</t>
+  </si>
+  <si>
+    <t>Rebecca Grier, Laura Freeman</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Grier, Rebecca A, and Laura Freeman. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Surveys in Operational Test &amp; Evaluation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document D-5410. Alexandria, VA: Institute for Defense Analyses, 2015.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wojton, Heather, Jonathan Snavely, and Justin Mary. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Introduction to Survey Design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-5835. Alexandria, VA: Institute for Defense Analyses, 2016.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Johnson, Thomas, Laura Freeman, and Raymond Chen. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tutorial on Sensitivity Testing in Live Fire Test and Evaluation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-5829. Alexandria, VA: Institute for Defense Analyses, 2016.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Avery, Matthew, Jonathan Bell, Rebecca Medlin, and Freeman Laura. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DOT&amp;E Reliability Course</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-5836. Alexandria, VA: Institute for Defense Analyses, 2016.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fronczyk, Kassandra. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bayesian Analysis in R/STAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-5831. Alexandria, VA: Institute for Defense Analyses, 2016.</t>
+    </r>
+  </si>
+  <si>
+    <t>Freeman, Laura, Pamela Rambow, and Jonathan Snavely. Science of Test Workshop Proceedings. IDA Document NS D-8249. Alexandria, VA: Institute for Defense Analyses, 2016.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Porter, Daniel, Emily Fedele, and Heather Wojton. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pilot Training Next: Modeling Skill Transfer in a Military Learning Environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-10927. Alexandria, VA: Institute for Defense Analyses, 2019.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wojton, Heather M, Keyla Pagan-Rivera, John T Haman, and Rebecca M Medlin. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Introduction to Bayesian Analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-20484. Alexandria, VA: Institute for Defense Analyses, 2021.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gilmore, James M, Kelly M Avery, Matthew R Girardi, and Rebecca M Medlin. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thoughts on Applying Design of Experiments (DOE) to Cyber Testing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. IDA Document NS D-33023. Alexandria, VA: Institute for Defense Analyses, 2022.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scientific Test and Analysis Techniques- Statistical Measures of Merit</t>
+  </si>
+  <si>
+    <t>Pilot Training Next- Modeling Skill Transfer in a Military Learning Environment</t>
+  </si>
+  <si>
+    <t>test and evaluation, Measures of Effectiveness</t>
+  </si>
+  <si>
+    <t>Bayesian analysis, Test Planning, Scientific Test and Analysis Techniques</t>
+  </si>
+  <si>
+    <t>Design of Experiments, statistical analyses, Test Planning, Statistical Measures of Merit</t>
+  </si>
+  <si>
+    <t>Defense Acquisition, Design of Experiments, experimental methods, AN/BQQ-10</t>
+  </si>
+  <si>
+    <t>personal protective equipment, combat helmets, statistical analyses</t>
+  </si>
+  <si>
+    <t>Surveys, Operational Test and Evaluation, Human Systems Interaction</t>
+  </si>
+  <si>
+    <t>Operational Testing, Design of Experiments, Live Fire Test and Evaluation, Sequential Design, Sensitivity Testing</t>
+  </si>
+  <si>
+    <t>Department of Defense, Reliability, Reliability Growth, Reliability Analysis, Test and Evaluation Master Plan</t>
+  </si>
+  <si>
+    <t>Air Force, Pilot Training Next (PTN), Simulators, pilot training, Linear Mixed Models</t>
+  </si>
+  <si>
+    <t>Cyber Assessments, Cyber Testing, Design of Experiments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4037,8 +4513,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4048,6 +4531,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -4060,10 +4548,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4110,9 +4599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4123,8 +4609,18 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4439,19 +4935,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L129" sqref="L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.86328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.86328125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.19921875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.9296875" style="7" customWidth="1"/>
     <col min="5" max="5" width="42" style="7" customWidth="1"/>
     <col min="6" max="6" width="31.46484375" style="2" customWidth="1"/>
     <col min="7" max="10" width="27.86328125" style="2"/>
@@ -4465,10 +4961,10 @@
       <c r="A1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="1" t="s">
         <v>440</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -4515,10 +5011,10 @@
       <c r="A2" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="17">
         <v>2009</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="2" t="s">
         <v>441</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -4547,10 +5043,10 @@
       <c r="A3" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="17">
         <v>2009</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="2" t="s">
         <v>441</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -4579,10 +5075,10 @@
       <c r="A4" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>2010</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="2" t="s">
         <v>442</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -4611,10 +5107,10 @@
       <c r="A5" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="17">
         <v>2011</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="2" t="s">
         <v>443</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -4646,10 +5142,10 @@
       <c r="A6" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="17">
         <v>2011</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="2" t="s">
         <v>444</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -4678,10 +5174,10 @@
       <c r="A7" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>2012</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="2" t="s">
         <v>445</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -4713,10 +5209,10 @@
       <c r="A8" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="17">
         <v>2013</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="2" t="s">
         <v>446</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -4748,10 +5244,10 @@
       <c r="A9" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>2013</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="2" t="s">
         <v>447</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -4780,10 +5276,10 @@
       <c r="A10" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <v>2014</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="2" t="s">
         <v>448</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -4812,10 +5308,10 @@
       <c r="A11" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>2014</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="2" t="s">
         <v>449</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -4844,10 +5340,10 @@
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <v>2015</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="2" t="s">
         <v>452</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -4876,10 +5372,10 @@
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="17">
         <v>2015</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="2" t="s">
         <v>453</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -4911,10 +5407,10 @@
       <c r="A14" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="17">
         <v>2015</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="2" t="s">
         <v>454</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -4943,10 +5439,10 @@
       <c r="A15" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="17">
         <v>2015</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="2" t="s">
         <v>451</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -4975,10 +5471,10 @@
       <c r="A16" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>2015</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="2" t="s">
         <v>450</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -5007,10 +5503,10 @@
       <c r="A17" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="17">
         <v>2016</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="2" t="s">
         <v>455</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -5039,10 +5535,10 @@
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="17">
         <v>2016</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="2" t="s">
         <v>456</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -5074,10 +5570,10 @@
       <c r="A19" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="17">
         <v>2016</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="2" t="s">
         <v>457</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -5106,10 +5602,10 @@
       <c r="A20" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="17">
         <v>2016</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="2" t="s">
         <v>458</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -5138,10 +5634,10 @@
       <c r="A21" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="17">
         <v>2017</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="2" t="s">
         <v>459</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -5174,10 +5670,10 @@
       <c r="A22" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="17">
         <v>2017</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="2" t="s">
         <v>460</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -5209,10 +5705,10 @@
       <c r="A23" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="17">
         <v>2017</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="2" t="s">
         <v>461</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -5244,10 +5740,10 @@
       <c r="A24" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="17">
         <v>2017</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="2" t="s">
         <v>455</v>
       </c>
       <c r="D24" s="7" t="s">
@@ -5276,10 +5772,10 @@
       <c r="A25" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="17">
         <v>2018</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="2" t="s">
         <v>464</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -5308,10 +5804,10 @@
       <c r="A26" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="17">
         <v>2018</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="2" t="s">
         <v>470</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -5340,10 +5836,10 @@
       <c r="A27" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="17">
         <v>2018</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="2" t="s">
         <v>467</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -5372,10 +5868,10 @@
       <c r="A28" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="17">
         <v>2018</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="2" t="s">
         <v>468</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -5407,10 +5903,10 @@
       <c r="A29" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="17">
         <v>2018</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="2" t="s">
         <v>466</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -5439,10 +5935,10 @@
       <c r="A30" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="17">
         <v>2018</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="2" t="s">
         <v>463</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -5471,10 +5967,10 @@
       <c r="A31" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="17">
         <v>2018</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="2" t="s">
         <v>462</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -5503,10 +5999,10 @@
       <c r="A32" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="17">
         <v>2018</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="2" t="s">
         <v>465</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -5535,10 +6031,10 @@
       <c r="A33" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="17">
         <v>2018</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="2" t="s">
         <v>469</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -5567,10 +6063,10 @@
       <c r="A34" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" s="17">
         <v>2019</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="2" t="s">
         <v>471</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -5602,10 +6098,10 @@
       <c r="A35" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="17">
         <v>2019</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="2" t="s">
         <v>473</v>
       </c>
       <c r="D35" s="7" t="s">
@@ -5634,10 +6130,10 @@
       <c r="A36" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="17">
         <v>2019</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="2" t="s">
         <v>474</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -5670,10 +6166,10 @@
       <c r="A37" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="17">
         <v>2019</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="2" t="s">
         <v>475</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -5708,10 +6204,10 @@
       <c r="A38" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="17">
         <v>2019</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="2" t="s">
         <v>477</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -5749,10 +6245,10 @@
       <c r="A39" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="17">
         <v>2019</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="2" t="s">
         <v>641</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -5781,10 +6277,10 @@
       <c r="A40" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="17">
         <v>2019</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="2" t="s">
         <v>484</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -5813,10 +6309,10 @@
       <c r="A41" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="17">
         <v>2019</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="2" t="s">
         <v>485</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -5848,10 +6344,10 @@
       <c r="A42" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="17">
         <v>2019</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="2" t="s">
         <v>480</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -5883,10 +6379,10 @@
       <c r="A43" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="17">
         <v>2019</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="2" t="s">
         <v>482</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -5918,10 +6414,10 @@
       <c r="A44" t="s">
         <v>367</v>
       </c>
-      <c r="B44" s="21">
+      <c r="B44" s="18">
         <v>2019</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="2" t="s">
         <v>478</v>
       </c>
       <c r="D44" t="s">
@@ -5936,6 +6432,7 @@
       <c r="H44" t="s">
         <v>429</v>
       </c>
+      <c r="I44" s="2"/>
       <c r="K44" t="s">
         <v>435</v>
       </c>
@@ -5950,10 +6447,10 @@
       <c r="A45" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="17">
         <v>2019</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="2" t="s">
         <v>472</v>
       </c>
       <c r="D45" s="7" t="s">
@@ -5982,10 +6479,10 @@
       <c r="A46" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B46" s="17">
         <v>2019</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="2" t="s">
         <v>476</v>
       </c>
       <c r="D46" s="7" t="s">
@@ -6014,10 +6511,10 @@
       <c r="A47" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B47" s="20">
+      <c r="B47" s="17">
         <v>2019</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="2" t="s">
         <v>481</v>
       </c>
       <c r="D47" s="7" t="s">
@@ -6046,10 +6543,10 @@
       <c r="A48" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" s="17">
         <v>2019</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="2" t="s">
         <v>483</v>
       </c>
       <c r="D48" s="7" t="s">
@@ -6078,10 +6575,10 @@
       <c r="A49" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B49" s="17">
         <v>2019</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="2" t="s">
         <v>486</v>
       </c>
       <c r="D49" s="7" t="s">
@@ -6113,10 +6610,10 @@
       <c r="A50" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="17">
         <v>2019</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="2" t="s">
         <v>479</v>
       </c>
       <c r="D50" s="7" t="s">
@@ -6145,10 +6642,10 @@
       <c r="A51" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="17">
         <v>2020</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="2" t="s">
         <v>487</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -6177,10 +6674,10 @@
       <c r="A52" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B52" s="20">
+      <c r="B52" s="17">
         <v>2020</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="2" t="s">
         <v>489</v>
       </c>
       <c r="D52" s="7" t="s">
@@ -6218,10 +6715,10 @@
       <c r="A53" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B53" s="20">
+      <c r="B53" s="17">
         <v>2020</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="2" t="s">
         <v>491</v>
       </c>
       <c r="D53" s="7" t="s">
@@ -6250,10 +6747,10 @@
       <c r="A54" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B54" s="20">
+      <c r="B54" s="17">
         <v>2020</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="2" t="s">
         <v>492</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -6285,10 +6782,10 @@
       <c r="A55" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" s="17">
         <v>2020</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="2" t="s">
         <v>653</v>
       </c>
       <c r="D55" s="7" t="s">
@@ -6320,10 +6817,10 @@
       <c r="A56" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" s="17">
         <v>2020</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="2" t="s">
         <v>488</v>
       </c>
       <c r="D56" s="7" t="s">
@@ -6355,10 +6852,10 @@
       <c r="A57" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" s="17">
         <v>2020</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="2" t="s">
         <v>490</v>
       </c>
       <c r="D57" s="7" t="s">
@@ -6387,10 +6884,10 @@
       <c r="A58" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B58" s="20">
+      <c r="B58" s="17">
         <v>2021</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="2" t="s">
         <v>493</v>
       </c>
       <c r="D58" s="7" t="s">
@@ -6416,10 +6913,10 @@
       <c r="A59" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B59" s="20">
+      <c r="B59" s="17">
         <v>2021</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="2" t="s">
         <v>494</v>
       </c>
       <c r="D59" s="7" t="s">
@@ -6448,10 +6945,10 @@
       <c r="A60" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B60" s="20">
+      <c r="B60" s="17">
         <v>2021</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="2" t="s">
         <v>497</v>
       </c>
       <c r="D60" s="7" t="s">
@@ -6483,10 +6980,10 @@
       <c r="A61" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" s="17">
         <v>2021</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="2" t="s">
         <v>499</v>
       </c>
       <c r="D61" s="7" t="s">
@@ -6515,10 +7012,10 @@
       <c r="A62" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B62" s="20">
+      <c r="B62" s="17">
         <v>2021</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="2" t="s">
         <v>495</v>
       </c>
       <c r="D62" s="7" t="s">
@@ -6550,10 +7047,10 @@
       <c r="A63" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B63" s="20">
+      <c r="B63" s="17">
         <v>2021</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="2" t="s">
         <v>498</v>
       </c>
       <c r="D63" s="7" t="s">
@@ -6585,10 +7082,10 @@
       <c r="A64" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="22">
+      <c r="B64" s="19">
         <v>2021</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="4" t="s">
         <v>496</v>
       </c>
       <c r="D64" s="10" t="s">
@@ -6615,10 +7112,10 @@
       <c r="A65" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B65" s="20">
+      <c r="B65" s="17">
         <v>2022</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="2" t="s">
         <v>500</v>
       </c>
       <c r="D65" s="7" t="s">
@@ -6653,10 +7150,10 @@
       <c r="A66" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" s="17">
         <v>2022</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="2" t="s">
         <v>503</v>
       </c>
       <c r="D66" s="7" t="s">
@@ -6691,10 +7188,10 @@
       <c r="A67" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B67" s="20">
+      <c r="B67" s="17">
         <v>2022</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C67" s="2" t="s">
         <v>504</v>
       </c>
       <c r="D67" s="7" t="s">
@@ -6723,10 +7220,10 @@
       <c r="A68" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" s="17">
         <v>2022</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="2" t="s">
         <v>505</v>
       </c>
       <c r="D68" s="7" t="s">
@@ -6758,10 +7255,10 @@
       <c r="A69" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B69" s="20">
+      <c r="B69" s="17">
         <v>2022</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C69" s="2" t="s">
         <v>502</v>
       </c>
       <c r="D69" s="7" t="s">
@@ -6793,10 +7290,10 @@
       <c r="A70" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B70" s="20">
+      <c r="B70" s="17">
         <v>2022</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C70" s="2" t="s">
         <v>467</v>
       </c>
       <c r="D70" s="7" t="s">
@@ -6828,10 +7325,10 @@
       <c r="A71" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B71" s="20">
+      <c r="B71" s="17">
         <v>2022</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C71" s="2" t="s">
         <v>501</v>
       </c>
       <c r="D71" s="7" t="s">
@@ -6863,10 +7360,10 @@
       <c r="A72" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B72" s="20">
+      <c r="B72" s="17">
         <v>2022</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="C72" s="2" t="s">
         <v>506</v>
       </c>
       <c r="D72" s="7" t="s">
@@ -6898,10 +7395,10 @@
       <c r="A73" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B73" s="20">
+      <c r="B73" s="17">
         <v>2023</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C73" s="2" t="s">
         <v>507</v>
       </c>
       <c r="D73" s="15" t="s">
@@ -6933,10 +7430,10 @@
       <c r="A74" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B74" s="20">
+      <c r="B74" s="17">
         <v>2023</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C74" s="2" t="s">
         <v>508</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -6965,10 +7462,10 @@
       <c r="A75" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B75" s="20">
+      <c r="B75" s="17">
         <v>2023</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="2" t="s">
         <v>510</v>
       </c>
       <c r="D75" s="7" t="s">
@@ -7000,10 +7497,10 @@
       <c r="A76" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B76" s="20">
+      <c r="B76" s="17">
         <v>2023</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="2" t="s">
         <v>511</v>
       </c>
       <c r="D76" s="7" t="s">
@@ -7032,10 +7529,10 @@
       <c r="A77" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B77" s="20">
+      <c r="B77" s="17">
         <v>2024</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="2" t="s">
         <v>522</v>
       </c>
       <c r="D77" s="7" t="s">
@@ -7070,10 +7567,10 @@
       <c r="A78" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" s="17">
         <v>2023</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="2" t="s">
         <v>512</v>
       </c>
       <c r="D78" s="7" t="s">
@@ -7108,10 +7605,10 @@
       <c r="A79" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B79" s="20">
+      <c r="B79" s="17">
         <v>2023</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="2" t="s">
         <v>514</v>
       </c>
       <c r="D79" s="7" t="s">
@@ -7143,10 +7640,10 @@
       <c r="A80" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="20">
+      <c r="B80" s="17">
         <v>2023</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="2" t="s">
         <v>515</v>
       </c>
       <c r="D80" s="7" t="s">
@@ -7175,10 +7672,10 @@
       <c r="A81" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B81" s="20">
+      <c r="B81" s="17">
         <v>2023</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C81" s="2" t="s">
         <v>516</v>
       </c>
       <c r="D81" s="7" t="s">
@@ -7210,10 +7707,10 @@
       <c r="A82" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B82" s="20">
+      <c r="B82" s="17">
         <v>2023</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="2" t="s">
         <v>518</v>
       </c>
       <c r="D82" s="7" t="s">
@@ -7248,10 +7745,10 @@
       <c r="A83" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B83" s="20">
+      <c r="B83" s="17">
         <v>2023</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="2" t="s">
         <v>501</v>
       </c>
       <c r="D83" s="7" t="s">
@@ -7283,10 +7780,10 @@
       <c r="A84" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B84" s="20">
+      <c r="B84" s="17">
         <v>2023</v>
       </c>
-      <c r="C84" s="17" t="s">
+      <c r="C84" s="2" t="s">
         <v>517</v>
       </c>
       <c r="D84" s="7" t="s">
@@ -7315,10 +7812,10 @@
       <c r="A85" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B85" s="20">
+      <c r="B85" s="17">
         <v>2023</v>
       </c>
-      <c r="C85" s="17" t="s">
+      <c r="C85" s="2" t="s">
         <v>509</v>
       </c>
       <c r="D85" s="7" t="s">
@@ -7353,10 +7850,10 @@
       <c r="A86" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B86" s="20">
+      <c r="B86" s="17">
         <v>2023</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C86" s="2" t="s">
         <v>513</v>
       </c>
       <c r="D86" s="7" t="s">
@@ -7385,10 +7882,10 @@
       <c r="A87" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B87" s="20">
+      <c r="B87" s="17">
         <v>2023</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C87" s="2" t="s">
         <v>519</v>
       </c>
       <c r="D87" s="7" t="s">
@@ -7417,10 +7914,10 @@
       <c r="A88" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B88" s="20">
+      <c r="B88" s="17">
         <v>2024</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C88" s="2" t="s">
         <v>523</v>
       </c>
       <c r="D88" s="7" t="s">
@@ -7452,10 +7949,10 @@
       <c r="A89" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B89" s="20">
+      <c r="B89" s="17">
         <v>2024</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="2" t="s">
         <v>524</v>
       </c>
       <c r="D89" s="7" t="s">
@@ -7487,10 +7984,10 @@
       <c r="A90" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B90" s="20">
+      <c r="B90" s="17">
         <v>2024</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="2" t="s">
         <v>501</v>
       </c>
       <c r="D90" s="7" t="s">
@@ -7522,10 +8019,10 @@
       <c r="A91" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B91" s="20">
+      <c r="B91" s="17">
         <v>2024</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="2" t="s">
         <v>525</v>
       </c>
       <c r="D91" s="7" t="s">
@@ -7554,10 +8051,10 @@
       <c r="A92" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B92" s="20">
+      <c r="B92" s="17">
         <v>2024</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="2" t="s">
         <v>526</v>
       </c>
       <c r="D92" s="7" t="s">
@@ -7595,10 +8092,10 @@
       <c r="A93" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B93" s="20">
+      <c r="B93" s="17">
         <v>2024</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C93" s="2" t="s">
         <v>520</v>
       </c>
       <c r="D93" s="7" t="s">
@@ -7630,10 +8127,10 @@
       <c r="A94" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B94" s="20">
+      <c r="B94" s="17">
         <v>2024</v>
       </c>
-      <c r="C94" s="17" t="s">
+      <c r="C94" s="2" t="s">
         <v>528</v>
       </c>
       <c r="D94" s="7" t="s">
@@ -7665,10 +8162,10 @@
       <c r="A95" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B95" s="20">
+      <c r="B95" s="17">
         <v>2024</v>
       </c>
-      <c r="C95" s="17" t="s">
+      <c r="C95" s="2" t="s">
         <v>521</v>
       </c>
       <c r="D95" s="7" t="s">
@@ -7697,10 +8194,10 @@
       <c r="A96" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B96" s="20">
+      <c r="B96" s="17">
         <v>2024</v>
       </c>
-      <c r="C96" s="17" t="s">
+      <c r="C96" s="2" t="s">
         <v>527</v>
       </c>
       <c r="D96" s="7" t="s">
@@ -7729,10 +8226,10 @@
       <c r="A97" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B97" s="20">
+      <c r="B97" s="17">
         <v>2017</v>
       </c>
-      <c r="C97" s="17" t="s">
+      <c r="C97" s="2" t="s">
         <v>455</v>
       </c>
       <c r="D97" s="7" t="s">
@@ -7761,10 +8258,10 @@
       <c r="A98" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B98" s="20">
+      <c r="B98" s="17">
         <v>2017</v>
       </c>
-      <c r="C98" s="17" t="s">
+      <c r="C98" s="2" t="s">
         <v>550</v>
       </c>
       <c r="D98" s="7" t="s">
@@ -7793,10 +8290,10 @@
       <c r="A99" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B99" s="20">
+      <c r="B99" s="17">
         <v>2011</v>
       </c>
-      <c r="C99" s="17" t="s">
+      <c r="C99" s="2" t="s">
         <v>462</v>
       </c>
       <c r="D99" s="7" t="s">
@@ -7825,10 +8322,10 @@
       <c r="A100" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B100" s="20">
+      <c r="B100" s="17">
         <v>2019</v>
       </c>
-      <c r="C100" s="17" t="s">
+      <c r="C100" s="2" t="s">
         <v>567</v>
       </c>
       <c r="D100" s="7" t="s">
@@ -7857,10 +8354,10 @@
       <c r="A101" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B101" s="20">
+      <c r="B101" s="17">
         <v>2018</v>
       </c>
-      <c r="C101" s="17" t="s">
+      <c r="C101" s="2" t="s">
         <v>571</v>
       </c>
       <c r="D101" s="7" t="s">
@@ -7889,10 +8386,10 @@
       <c r="A102" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B102" s="20">
+      <c r="B102" s="17">
         <v>2013</v>
       </c>
-      <c r="C102" s="17" t="s">
+      <c r="C102" s="2" t="s">
         <v>457</v>
       </c>
       <c r="D102" s="2" t="s">
@@ -7921,10 +8418,10 @@
       <c r="A103" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B103" s="20">
+      <c r="B103" s="17">
         <v>2017</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="2" t="s">
         <v>457</v>
       </c>
       <c r="D103" s="7" t="s">
@@ -7953,10 +8450,10 @@
       <c r="A104" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B104" s="20">
+      <c r="B104" s="17">
         <v>2011</v>
       </c>
-      <c r="C104" s="17" t="s">
+      <c r="C104" s="2" t="s">
         <v>462</v>
       </c>
       <c r="D104" s="7" t="s">
@@ -7985,10 +8482,10 @@
       <c r="A105" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B105" s="20">
+      <c r="B105" s="17">
         <v>2011</v>
       </c>
-      <c r="C105" s="17" t="s">
+      <c r="C105" s="2" t="s">
         <v>587</v>
       </c>
       <c r="D105" s="7" t="s">
@@ -8017,10 +8514,10 @@
       <c r="A106" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B106" s="20">
+      <c r="B106" s="17">
         <v>2012</v>
       </c>
-      <c r="C106" s="17" t="s">
+      <c r="C106" s="2" t="s">
         <v>462</v>
       </c>
       <c r="D106" s="2" t="s">
@@ -8049,10 +8546,10 @@
       <c r="A107" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B107" s="20">
+      <c r="B107" s="17">
         <v>2014</v>
       </c>
-      <c r="C107" s="17" t="s">
+      <c r="C107" s="2" t="s">
         <v>593</v>
       </c>
       <c r="D107" s="7" t="s">
@@ -8081,10 +8578,10 @@
       <c r="A108" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B108" s="20">
+      <c r="B108" s="17">
         <v>2017</v>
       </c>
-      <c r="C108" s="17" t="s">
+      <c r="C108" s="2" t="s">
         <v>597</v>
       </c>
       <c r="D108" s="7" t="s">
@@ -8113,10 +8610,10 @@
       <c r="A109" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B109" s="20">
+      <c r="B109" s="17">
         <v>2017</v>
       </c>
-      <c r="C109" s="17" t="s">
+      <c r="C109" s="2" t="s">
         <v>601</v>
       </c>
       <c r="D109" s="7" t="s">
@@ -8145,10 +8642,10 @@
       <c r="A110" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B110" s="20">
+      <c r="B110" s="17">
         <v>2017</v>
       </c>
-      <c r="C110" s="17" t="s">
+      <c r="C110" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D110" s="7" t="s">
@@ -8177,10 +8674,10 @@
       <c r="A111" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B111" s="20">
+      <c r="B111" s="17">
         <v>2016</v>
       </c>
-      <c r="C111" s="17" t="s">
+      <c r="C111" s="2" t="s">
         <v>462</v>
       </c>
       <c r="D111" s="7" t="s">
@@ -8209,10 +8706,10 @@
       <c r="A112" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B112" s="20">
+      <c r="B112" s="17">
         <v>2018</v>
       </c>
-      <c r="C112" s="17" t="s">
+      <c r="C112" s="2" t="s">
         <v>610</v>
       </c>
       <c r="D112" s="7" t="s">
@@ -8241,10 +8738,10 @@
       <c r="A113" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B113" s="20">
+      <c r="B113" s="17">
         <v>2024</v>
       </c>
-      <c r="C113" s="17" t="s">
+      <c r="C113" s="2" t="s">
         <v>527</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -8273,7 +8770,7 @@
       <c r="A114" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B114" s="20">
+      <c r="B114" s="17">
         <v>2018</v>
       </c>
       <c r="C114" s="2" t="s">
@@ -8305,7 +8802,7 @@
       <c r="A115" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B115" s="20">
+      <c r="B115" s="17">
         <v>2018</v>
       </c>
       <c r="C115" s="2" t="s">
@@ -8330,6 +8827,458 @@
         <v>685</v>
       </c>
       <c r="M115" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A116" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B116" s="21">
+        <v>2012</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="D116" s="22" t="s">
+        <v>780</v>
+      </c>
+      <c r="E116" s="22" t="s">
+        <v>835</v>
+      </c>
+      <c r="F116" s="20" t="s">
+        <v>576</v>
+      </c>
+      <c r="I116" s="20" t="s">
+        <v>781</v>
+      </c>
+      <c r="K116" s="20" t="s">
+        <v>782</v>
+      </c>
+      <c r="L116" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="M116" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>338</v>
+      </c>
+      <c r="B117">
+        <v>2012</v>
+      </c>
+      <c r="C117" t="s">
+        <v>783</v>
+      </c>
+      <c r="D117" t="s">
+        <v>784</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>836</v>
+      </c>
+      <c r="F117" t="s">
+        <v>563</v>
+      </c>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="J117" s="2"/>
+      <c r="K117" t="s">
+        <v>786</v>
+      </c>
+      <c r="L117" t="s">
+        <v>853</v>
+      </c>
+      <c r="M117" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>338</v>
+      </c>
+      <c r="B118">
+        <v>2013</v>
+      </c>
+      <c r="C118" t="s">
+        <v>462</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="E118" t="s">
+        <v>837</v>
+      </c>
+      <c r="F118" t="s">
+        <v>655</v>
+      </c>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="J118" s="2"/>
+      <c r="K118" t="s">
+        <v>787</v>
+      </c>
+      <c r="L118" t="s">
+        <v>854</v>
+      </c>
+      <c r="M118" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A119" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B119" s="17">
+        <v>2014</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="M119" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B120" s="17">
+        <v>2014</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A121" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B121" s="17">
+        <v>2015</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="M121" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B122" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="E122" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="M122" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A123" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B123" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>843</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="M123" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A124" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B124" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="E124" s="12" t="s">
+        <v>844</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="M124" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A125" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B125" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="E125" s="12" t="s">
+        <v>845</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A126" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B126" s="17">
+        <v>2016</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="M126" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A127" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" s="17">
+        <v>2019</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="E127" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="M127" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A128" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B128" s="17">
+        <v>2021</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>848</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="K128" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="M128" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A129" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B129" s="17">
+        <v>2022</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="E129" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="K129" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="L129" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="M129" s="2" t="s">
         <v>390</v>
       </c>
     </row>
@@ -8491,9 +9440,23 @@
     <hyperlink ref="E23" r:id="rId139" display="https://doi.org/10.1002/9781118445112.stat07946" xr:uid="{35A59AA7-19B1-4907-B821-794F8385D5FE}"/>
     <hyperlink ref="E49" r:id="rId140" display="https://www.jasp-online.org/asjournal/summer-2019/designs-of-experiments-doe-in-survivability-testing/" xr:uid="{F359D08E-AE8E-4916-B29B-49D1A002D119}"/>
     <hyperlink ref="E114" r:id="rId141" display="https://doi.org/10.1002/9781119357056.ch18" xr:uid="{933D4C61-B842-46E8-8C85-EF0A66C5F2F1}"/>
+    <hyperlink ref="I116" r:id="rId142" xr:uid="{97900ACB-1389-471A-ADBF-4279F8C6E079}"/>
+    <hyperlink ref="I117" r:id="rId143" xr:uid="{293EFF17-5C8A-43D4-92F4-B936C9A4FFCF}"/>
+    <hyperlink ref="I119" r:id="rId144" xr:uid="{E7FF5511-47A7-44F4-8BAE-76BF462A84B5}"/>
+    <hyperlink ref="I120" r:id="rId145" xr:uid="{E4F6C9F0-EEE5-4957-A4B0-5C6472FBD1E0}"/>
+    <hyperlink ref="I121" r:id="rId146" xr:uid="{CD58E132-90CE-4D9E-8EB0-4994BD4B4DD0}"/>
+    <hyperlink ref="I122" r:id="rId147" xr:uid="{E023AE51-5D3A-4343-B42D-1334FD9C0537}"/>
+    <hyperlink ref="I123" r:id="rId148" xr:uid="{9B603483-4809-4BB3-870B-B9FE8BA25F47}"/>
+    <hyperlink ref="I125" r:id="rId149" xr:uid="{868D39C9-F39F-4DA1-A5B6-80B53DD95CAF}"/>
+    <hyperlink ref="G126" r:id="rId150" xr:uid="{1A2C7A7A-0B11-4784-A570-D418C79BB6E3}"/>
+    <hyperlink ref="I127" r:id="rId151" xr:uid="{150786E4-33D6-4591-9CE0-7C18E79AD677}"/>
+    <hyperlink ref="I128" r:id="rId152" xr:uid="{4A038D1D-787F-4824-8754-DD691C1591B0}"/>
+    <hyperlink ref="I129" r:id="rId153" xr:uid="{715140CD-EFAD-4585-A4A0-6B2A814345FB}"/>
+    <hyperlink ref="I124" r:id="rId154" xr:uid="{25B3703B-F3C1-4A99-99A5-253F7CF04E55}"/>
+    <hyperlink ref="I118" r:id="rId155" xr:uid="{1410D822-9320-4241-84AA-6547A6022A3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId142"/>
+  <pageSetup orientation="portrait" r:id="rId156"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix non-breaking space char in xlsx
</commit_message>
<xml_diff>
--- a/test-science-documents-library.xlsx
+++ b/test-science-documents-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhaman\Documents\test-science-documents-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58F746F-7647-4948-A16F-BD96757BE1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C3513-4F94-4695-954E-D1C5A7CFC9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="624" windowWidth="18336" windowHeight="7536" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
+    <workbookView xWindow="30612" yWindow="348" windowWidth="30936" windowHeight="17040" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1397,9 +1397,6 @@
     <t>Heather Wojton, Daniel Porter, Stephanie Lane, Chad Bieber, Poornima Madhavan</t>
   </si>
   <si>
-    <t>Brent Crabtree, Andrew Cseko, Tom Johnson, Joel Williamson, Kelly Avery</t>
-  </si>
-  <si>
     <t>Heather Wojton, Daniel Porter, Yevgeniya Pinelis, Chad Bieber, Michael McAnally, Laura Freeman</t>
   </si>
   <si>
@@ -1953,9 +1950,6 @@
   </si>
   <si>
     <t>Johnson, Thomas H., Dhruv K. Patel, John T. Haman, Jeremy S. Werner, and Dave Higdon. “Uncertainty Quantification for Ground Vehicle Vulnerability Simulation.” Quality Engineering, August 19, 2024. https://www.tandfonline.com/doi/abs/10.1080/08982112.2024.2394437.</t>
-  </si>
-  <si>
-    <t>Laura Freeman, Thomas Johnson, Matthew Avery, V. Bram Lillard, Justace Clutter</t>
   </si>
   <si>
     <t>Testing Defense Systems</t>
@@ -4483,6 +4477,12 @@
   </si>
   <si>
     <t xml:space="preserve"> In today’s fiscal environment, efficient and effective testing is essential. Often, military system requirements are defined using probability of success as the primary measure of effectiveness – for example, a system must complete its mission 80 percent of the time; or the system must detect 90 percent of targets. The traditional approach to testing these probability-based requirements is to execute a series of trials and then total the number of successes; the ratio of successes to number of trails provides an intuitive measure of the probability of success. However, this method of testing has proven to be cost prohibitive, especially at high levels of statistical confidence and power. Often, one or more continuous metrics empirically related to the probability based metric provide more information about system performance than the pass/fail construct. Using these metrics in lieu of the probability-based metrics to plan testing both reduces test costs and provides a better understanding of system performance. In this talk the authors discusses the cost of using binary test metrics (e.g., success or failure, hit or miss). They present several common T&amp;E examples, translating the original probability based requirement to a related continuous metric, and show potential cost savings and information gain achieved by the conversion.</t>
+  </si>
+  <si>
+    <t>Brent Crabtree, Andrew Cseko, Thomas Johnson, Joel Williamson, Kelly Avery</t>
+  </si>
+  <si>
+    <t>Justace Clutter, Thomas Johnson, Matthew Avery, V. Bram Lillard, Laura Freeman</t>
   </si>
 </sst>
 </file>
@@ -4556,7 +4556,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4605,6 +4605,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4923,9 +4926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4957,10 +4960,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -4990,7 +4993,7 @@
         <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -5007,7 +5010,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>379</v>
@@ -5039,10 +5042,10 @@
         <v>72</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>73</v>
@@ -5071,10 +5074,10 @@
         <v>83</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>85</v>
@@ -5103,7 +5106,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>235</v>
@@ -5138,10 +5141,10 @@
         <v>310</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>87</v>
@@ -5170,7 +5173,7 @@
         <v>68</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>235</v>
@@ -5199,13 +5202,13 @@
         <v>2013</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>235</v>
@@ -5240,7 +5243,7 @@
         <v>158</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>235</v>
@@ -5272,7 +5275,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>380</v>
@@ -5304,10 +5307,10 @@
         <v>128</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>126</v>
@@ -5336,10 +5339,10 @@
         <v>93</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>94</v>
@@ -5348,7 +5351,7 @@
         <v>95</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>376</v>
@@ -5368,7 +5371,7 @@
         <v>138</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>381</v>
@@ -5380,7 +5383,7 @@
         <v>139</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>279</v>
@@ -5403,16 +5406,16 @@
         <v>161</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>162</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>163</v>
@@ -5435,10 +5438,10 @@
         <v>271</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>164</v>
@@ -5467,10 +5470,10 @@
         <v>170</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>166</v>
@@ -5499,10 +5502,10 @@
         <v>11</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>12</v>
@@ -5531,7 +5534,7 @@
         <v>311</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>235</v>
@@ -5566,7 +5569,7 @@
         <v>312</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>407</v>
@@ -5598,10 +5601,10 @@
         <v>129</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>130</v>
@@ -5630,10 +5633,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>16</v>
@@ -5666,7 +5669,7 @@
         <v>123</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>235</v>
@@ -5675,7 +5678,7 @@
         <v>125</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>124</v>
@@ -5701,10 +5704,10 @@
         <v>134</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>135</v>
@@ -5736,10 +5739,10 @@
         <v>175</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>176</v>
@@ -5768,7 +5771,7 @@
         <v>98</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>413</v>
@@ -5800,16 +5803,16 @@
         <v>178</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>179</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>285</v>
@@ -5832,7 +5835,7 @@
         <v>242</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>407</v>
@@ -5841,7 +5844,7 @@
         <v>182</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>286</v>
@@ -5864,13 +5867,13 @@
         <v>194</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>195</v>
@@ -5879,7 +5882,7 @@
         <v>387</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>377</v>
@@ -5899,16 +5902,16 @@
         <v>196</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>197</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>287</v>
@@ -5931,10 +5934,10 @@
         <v>313</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>245</v>
@@ -5963,10 +5966,10 @@
         <v>253</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>252</v>
@@ -5995,19 +5998,19 @@
         <v>254</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>255</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>256</v>
@@ -6027,19 +6030,19 @@
         <v>442</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>257</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>290</v>
@@ -6062,7 +6065,7 @@
         <v>48</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>235</v>
@@ -6080,7 +6083,7 @@
         <v>376</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -6097,10 +6100,10 @@
         <v>314</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>66</v>
@@ -6129,17 +6132,17 @@
         <v>315</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>70</v>
       </c>
       <c r="I36" s="4"/>
       <c r="K36" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>71</v>
@@ -6148,7 +6151,7 @@
         <v>375</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -6165,10 +6168,10 @@
         <v>92</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>86</v>
@@ -6203,10 +6206,10 @@
         <v>102</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>606</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>105</v>
@@ -6238,22 +6241,22 @@
         <v>2019</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>117</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>118</v>
@@ -6270,16 +6273,16 @@
         <v>2019</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>316</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>142</v>
@@ -6302,16 +6305,16 @@
         <v>2019</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>145</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>107</v>
@@ -6320,7 +6323,7 @@
         <v>107</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>146</v>
@@ -6337,13 +6340,13 @@
         <v>2019</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>155</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>407</v>
@@ -6352,7 +6355,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>388</v>
@@ -6372,13 +6375,13 @@
         <v>2019</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>171</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>407</v>
@@ -6387,7 +6390,7 @@
         <v>172</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>173</v>
@@ -6407,13 +6410,13 @@
         <v>2019</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>451</v>
+        <v>856</v>
       </c>
       <c r="D44" t="s">
         <v>404</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="F44" t="s">
         <v>407</v>
@@ -6423,7 +6426,7 @@
       </c>
       <c r="I44" s="2"/>
       <c r="K44" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="L44" t="s">
         <v>406</v>
@@ -6446,7 +6449,7 @@
         <v>317</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>407</v>
@@ -6458,7 +6461,7 @@
         <v>389</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>377</v>
@@ -6478,7 +6481,7 @@
         <v>241</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>407</v>
@@ -6487,7 +6490,7 @@
         <v>185</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>186</v>
@@ -6504,22 +6507,22 @@
         <v>2019</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>216</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>187</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>188</v>
@@ -6536,13 +6539,13 @@
         <v>2019</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>189</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>407</v>
@@ -6551,7 +6554,7 @@
         <v>190</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>295</v>
@@ -6568,13 +6571,13 @@
         <v>2019</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>246</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>228</v>
@@ -6583,10 +6586,10 @@
         <v>247</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>375</v>
@@ -6603,25 +6606,25 @@
         <v>2019</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>258</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>259</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>376</v>
@@ -6635,22 +6638,22 @@
         <v>2020</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>296</v>
@@ -6667,16 +6670,16 @@
         <v>2020</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E52" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>617</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>618</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>54</v>
@@ -6688,7 +6691,7 @@
         <v>157</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>56</v>
@@ -6708,25 +6711,25 @@
         <v>2020</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>318</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>141</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>375</v>
@@ -6740,16 +6743,16 @@
         <v>2020</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>319</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>147</v>
@@ -6758,10 +6761,10 @@
         <v>408</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>375</v>
@@ -6775,16 +6778,16 @@
         <v>2020</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>320</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>156</v>
@@ -6793,7 +6796,7 @@
         <v>152</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>297</v>
@@ -6810,13 +6813,13 @@
         <v>2020</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>321</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>407</v>
@@ -6828,7 +6831,7 @@
         <v>364</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>335</v>
@@ -6845,16 +6848,16 @@
         <v>2020</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>261</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>260</v>
@@ -6877,16 +6880,16 @@
         <v>2021</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>37</v>
@@ -6906,16 +6909,16 @@
         <v>2021</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>322</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>409</v>
@@ -6938,16 +6941,16 @@
         <v>2021</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>114</v>
@@ -6973,16 +6976,16 @@
         <v>2021</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>148</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>149</v>
@@ -7005,13 +7008,13 @@
         <v>2021</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>198</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>407</v>
@@ -7020,10 +7023,10 @@
         <v>199</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>298</v>
@@ -7040,22 +7043,22 @@
         <v>2021</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>200</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>201</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>339</v>
@@ -7064,7 +7067,7 @@
         <v>376</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7075,13 +7078,13 @@
         <v>2022</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>235</v>
@@ -7113,16 +7116,16 @@
         <v>2022</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>120</v>
@@ -7134,7 +7137,7 @@
         <v>122</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>341</v>
@@ -7151,16 +7154,16 @@
         <v>2022</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>191</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>192</v>
@@ -7183,13 +7186,13 @@
         <v>2022</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>202</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>407</v>
@@ -7218,13 +7221,13 @@
         <v>2022</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>323</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>407</v>
@@ -7236,7 +7239,7 @@
         <v>373</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>309</v>
@@ -7259,10 +7262,10 @@
         <v>237</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>238</v>
@@ -7271,7 +7274,7 @@
         <v>239</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>343</v>
@@ -7288,13 +7291,13 @@
         <v>2022</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>272</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>407</v>
@@ -7303,7 +7306,7 @@
         <v>248</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>400</v>
@@ -7323,13 +7326,13 @@
         <v>2022</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>262</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>407</v>
@@ -7358,16 +7361,16 @@
         <v>2023</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D72" s="14" t="s">
         <v>23</v>
       </c>
       <c r="E72" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>629</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>25</v>
@@ -7376,7 +7379,7 @@
         <v>26</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>24</v>
@@ -7396,22 +7399,22 @@
         <v>2023</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>29</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>292</v>
@@ -7428,13 +7431,13 @@
         <v>2023</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>407</v>
@@ -7463,16 +7466,16 @@
         <v>2023</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>64</v>
@@ -7495,16 +7498,16 @@
         <v>2024</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>324</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>75</v>
@@ -7533,16 +7536,16 @@
         <v>2023</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>81</v>
@@ -7554,7 +7557,7 @@
         <v>367</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>301</v>
@@ -7571,16 +7574,16 @@
         <v>2023</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>89</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>90</v>
@@ -7606,16 +7609,16 @@
         <v>2023</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>325</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>96</v>
@@ -7638,16 +7641,16 @@
         <v>2023</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>411</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>108</v>
@@ -7673,13 +7676,13 @@
         <v>2023</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>407</v>
@@ -7711,16 +7714,16 @@
         <v>2023</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>132</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>131</v>
@@ -7746,13 +7749,13 @@
         <v>2023</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>326</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>407</v>
@@ -7761,7 +7764,7 @@
         <v>204</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>329</v>
@@ -7778,13 +7781,13 @@
         <v>2023</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>225</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>228</v>
@@ -7796,7 +7799,7 @@
         <v>226</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>305</v>
@@ -7816,13 +7819,13 @@
         <v>2023</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>327</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>407</v>
@@ -7848,16 +7851,16 @@
         <v>2023</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>328</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I86" s="3" t="s">
         <v>243</v>
@@ -7880,13 +7883,13 @@
         <v>2024</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>167</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>407</v>
@@ -7915,13 +7918,13 @@
         <v>2024</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>205</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>407</v>
@@ -7933,7 +7936,7 @@
         <v>369</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>207</v>
@@ -7950,13 +7953,13 @@
         <v>2024</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>208</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>407</v>
@@ -7985,13 +7988,13 @@
         <v>2024</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>212</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>229</v>
@@ -8017,13 +8020,13 @@
         <v>2024</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>217</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>407</v>
@@ -8058,13 +8061,13 @@
         <v>2024</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>223</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>407</v>
@@ -8093,13 +8096,13 @@
         <v>2024</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>231</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>235</v>
@@ -8128,22 +8131,22 @@
         <v>2024</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>249</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>251</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>250</v>
@@ -8160,13 +8163,13 @@
         <v>2024</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>264</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>407</v>
@@ -8195,22 +8198,22 @@
         <v>428</v>
       </c>
       <c r="D96" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="I96" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="E96" s="11" t="s">
-        <v>733</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="I96" s="2" t="s">
+      <c r="K96" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="L96" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="K96" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="L96" s="2" t="s">
-        <v>515</v>
       </c>
       <c r="M96" s="2" t="s">
         <v>377</v>
@@ -8224,25 +8227,25 @@
         <v>2017</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="I97" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D97" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>734</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>518</v>
-      </c>
       <c r="K97" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>375</v>
@@ -8259,22 +8262,22 @@
         <v>435</v>
       </c>
       <c r="D98" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>733</v>
+      </c>
+      <c r="F98" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="E98" s="11" t="s">
-        <v>735</v>
-      </c>
-      <c r="F98" s="2" t="s">
+      <c r="I98" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="K98" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="K98" s="2" t="s">
+      <c r="L98" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="L98" s="2" t="s">
-        <v>532</v>
       </c>
       <c r="M98" s="2" t="s">
         <v>375</v>
@@ -8288,25 +8291,25 @@
         <v>2019</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D99" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="D99" s="7" t="s">
-        <v>534</v>
-      </c>
       <c r="E99" s="11" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>407</v>
       </c>
       <c r="I99" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="K99" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="L99" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="K99" s="10" t="s">
-        <v>663</v>
-      </c>
-      <c r="L99" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="M99" s="2" t="s">
         <v>376</v>
@@ -8320,25 +8323,25 @@
         <v>2018</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D100" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>538</v>
-      </c>
       <c r="E100" s="11" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>407</v>
       </c>
       <c r="H100" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="K100" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="L100" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="K100" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="L100" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="M100" s="2" t="s">
         <v>376</v>
@@ -8355,22 +8358,22 @@
         <v>430</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>736</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="E101" s="11" t="s">
-        <v>738</v>
-      </c>
-      <c r="F101" s="2" t="s">
+      <c r="I101" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="K101" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="K101" s="2" t="s">
+      <c r="L101" s="2" t="s">
         <v>544</v>
-      </c>
-      <c r="L101" s="2" t="s">
-        <v>545</v>
       </c>
       <c r="M101" s="2" t="s">
         <v>376</v>
@@ -8387,22 +8390,22 @@
         <v>430</v>
       </c>
       <c r="D102" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>737</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="I102" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E102" s="11" t="s">
-        <v>739</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="I102" s="2" t="s">
+      <c r="K102" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="L102" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="L102" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>375</v>
@@ -8419,22 +8422,22 @@
         <v>435</v>
       </c>
       <c r="D103" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>738</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="I103" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="E103" s="11" t="s">
-        <v>740</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="I103" s="2" t="s">
+      <c r="K103" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="L103" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="M103" s="2" t="s">
         <v>376</v>
@@ -8448,25 +8451,25 @@
         <v>2011</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="D104" s="7" t="s">
         <v>553</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="E104" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="K104" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="E104" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>555</v>
-      </c>
       <c r="L104" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M104" s="2" t="s">
         <v>375</v>
@@ -8483,22 +8486,22 @@
         <v>435</v>
       </c>
       <c r="D105" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>739</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E105" s="11" t="s">
-        <v>741</v>
-      </c>
-      <c r="F105" s="2" t="s">
+      <c r="I105" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>558</v>
-      </c>
       <c r="K105" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>375</v>
@@ -8512,25 +8515,25 @@
         <v>2014</v>
       </c>
       <c r="C106" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="E106" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="L106" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="L106" s="2" t="s">
-        <v>561</v>
       </c>
       <c r="M106" s="2" t="s">
         <v>375</v>
@@ -8544,25 +8547,25 @@
         <v>2017</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="D107" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="E107" s="11" t="s">
+        <v>740</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I107" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="E107" s="11" t="s">
-        <v>742</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I107" s="2" t="s">
+      <c r="K107" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="L107" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="L107" s="2" t="s">
-        <v>566</v>
       </c>
       <c r="M107" s="2" t="s">
         <v>375</v>
@@ -8576,25 +8579,25 @@
         <v>2017</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>235</v>
       </c>
       <c r="G108" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="K108" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="L108" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="K108" s="10" t="s">
-        <v>672</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>569</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>377</v>
@@ -8608,25 +8611,25 @@
         <v>2017</v>
       </c>
       <c r="C109" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="D109" s="7" t="s">
         <v>570</v>
       </c>
-      <c r="D109" s="7" t="s">
-        <v>571</v>
-      </c>
       <c r="E109" s="11" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>407</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M109" s="2" t="s">
         <v>376</v>
@@ -8643,22 +8646,22 @@
         <v>435</v>
       </c>
       <c r="D110" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>657</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="G110" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="E110" s="11" t="s">
-        <v>659</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="G110" s="2" t="s">
+      <c r="K110" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="L110" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="L110" s="2" t="s">
-        <v>575</v>
       </c>
       <c r="M110" s="2" t="s">
         <v>375</v>
@@ -8672,25 +8675,25 @@
         <v>2018</v>
       </c>
       <c r="C111" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="D111" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="E111" s="11" t="s">
+        <v>742</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="I111" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E111" s="11" t="s">
-        <v>744</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="I111" s="2" t="s">
+      <c r="K111" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="L111" s="2" t="s">
         <v>578</v>
-      </c>
-      <c r="K111" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="L111" s="2" t="s">
-        <v>579</v>
       </c>
       <c r="M111" s="2" t="s">
         <v>375</v>
@@ -8704,25 +8707,25 @@
         <v>2024</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>743</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I112" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E112" s="11" t="s">
-        <v>745</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I112" s="2" t="s">
+      <c r="K112" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="K112" s="2" t="s">
+      <c r="L112" s="2" t="s">
         <v>582</v>
-      </c>
-      <c r="L112" s="2" t="s">
-        <v>583</v>
       </c>
       <c r="M112" s="2" t="s">
         <v>375</v>
@@ -8735,23 +8738,23 @@
       <c r="B113" s="16">
         <v>2018</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="18" t="s">
+        <v>857</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="E113" s="12" t="s">
         <v>637</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="F113" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="E113" s="12" t="s">
+      <c r="G113" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="K113" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="K113" s="2" t="s">
-        <v>642</v>
       </c>
       <c r="L113" s="2" t="s">
         <v>299</v>
@@ -8768,25 +8771,25 @@
         <v>2018</v>
       </c>
       <c r="C114" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G114" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="E114" s="7" t="s">
+      <c r="K114" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="G114" s="3" t="s">
+      <c r="L114" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="K114" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="L114" s="2" t="s">
-        <v>651</v>
       </c>
       <c r="M114" s="2" t="s">
         <v>376</v>
@@ -8800,26 +8803,26 @@
         <v>2012</v>
       </c>
       <c r="C115" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D115" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E115" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F115" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H115" s="2"/>
       <c r="I115" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="K115" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="L115" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="M115" t="s">
         <v>375</v>
@@ -8833,27 +8836,27 @@
         <v>2012</v>
       </c>
       <c r="C116" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D116" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F116" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J116" s="2"/>
       <c r="K116" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="L116" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="M116" t="s">
         <v>375</v>
@@ -8870,24 +8873,24 @@
         <v>435</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E117" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F117" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J117" s="2"/>
       <c r="K117" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="L117" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="M117" t="s">
         <v>375</v>
@@ -8901,25 +8904,25 @@
         <v>2014</v>
       </c>
       <c r="C118" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="K118" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>754</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>796</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="K118" s="2" t="s">
-        <v>757</v>
-      </c>
       <c r="L118" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="M118" s="2" t="s">
         <v>375</v>
@@ -8933,25 +8936,25 @@
         <v>2014</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D119" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I119" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="E119" s="7" t="s">
-        <v>797</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>760</v>
-      </c>
       <c r="K119" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="M119" s="2" t="s">
         <v>376</v>
@@ -8965,25 +8968,25 @@
         <v>2015</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="M120" s="2" t="s">
         <v>375</v>
@@ -8997,25 +9000,25 @@
         <v>2016</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="L121" s="2" t="s">
         <v>764</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="E121" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I121" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="K121" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="L121" s="2" t="s">
-        <v>766</v>
       </c>
       <c r="M121" s="2" t="s">
         <v>375</v>
@@ -9029,25 +9032,25 @@
         <v>2016</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I122" s="3" t="s">
         <v>767</v>
       </c>
-      <c r="E122" s="11" t="s">
-        <v>801</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>769</v>
-      </c>
       <c r="K122" s="2" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="M122" s="2" t="s">
         <v>376</v>
@@ -9061,25 +9064,25 @@
         <v>2016</v>
       </c>
       <c r="C123" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>800</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="K123" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>773</v>
-      </c>
-      <c r="E123" s="11" t="s">
-        <v>802</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="K123" s="2" t="s">
-        <v>772</v>
-      </c>
       <c r="L123" s="2" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="M123" s="2" t="s">
         <v>375</v>
@@ -9093,25 +9096,25 @@
         <v>2016</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>407</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="M124" s="2" t="s">
         <v>375</v>
@@ -9125,25 +9128,25 @@
         <v>2016</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>407</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M125" s="2" t="s">
         <v>375</v>
@@ -9157,25 +9160,25 @@
         <v>2019</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="M126" s="2" t="s">
         <v>375</v>
@@ -9189,25 +9192,25 @@
         <v>2021</v>
       </c>
       <c r="C127" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>804</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I127" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="K127" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="L127" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="E127" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>788</v>
-      </c>
-      <c r="K127" s="2" t="s">
-        <v>850</v>
-      </c>
-      <c r="L127" s="2" t="s">
-        <v>787</v>
       </c>
       <c r="M127" s="2" t="s">
         <v>376</v>
@@ -9221,25 +9224,25 @@
         <v>2022</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>407</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="M128" s="2" t="s">
         <v>376</v>

</xml_diff>

<commit_message>
Hide Cover Images for now.
They look a little bit tacky, but maybe there is a better way to do this.
</commit_message>
<xml_diff>
--- a/test-science-documents-library.xlsx
+++ b/test-science-documents-library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhaman\Documents\test-science-documents-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C3513-4F94-4695-954E-D1C5A7CFC9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4069E74B-7678-4BD1-8396-2C33BC0B9AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="348" windowWidth="30936" windowHeight="17040" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="864">
   <si>
     <t>Project</t>
   </si>
@@ -4483,6 +4483,25 @@
   </si>
   <si>
     <t>Justace Clutter, Thomas Johnson, Matthew Avery, V. Bram Lillard, Laura Freeman</t>
+  </si>
+  <si>
+    <t>Paper-Citation</t>
+  </si>
+  <si>
+    <t>Poster-Citation</t>
+  </si>
+  <si>
+    <t>Slides-Citation</t>
+  </si>
+  <si>
+    <t>Adam Miller, Keyla Pagan-Rivera</t>
+  </si>
+  <si>
+    <t>Introduction to Human-Systems Interaction in Operational Test and Evaluation Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    Human-System Interaction (HSI) is the study of interfaces between humans and technical systems. The Department of Defense incorporates HSI evaluations into defense acquisition to improve system performance and reduce lifecycle costs. During operational test and evaluation, HSI evaluations characterize how a system’s operational performance is affected by its users. The goal of this course is to provide the theoretical background and practical tools necessary to plan and evaluate HSI test plans, collect and analyze HSI data, and report on HSI results. We will discuss HSI concepts, measurement methods, design of experiments, data analysis, and evaluation and reporting, all from an operational testing perspective. </t>
   </si>
 </sst>
 </file>
@@ -4924,11 +4943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:S129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T129" sqref="T129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4939,14 +4958,14 @@
     <col min="4" max="4" width="39.21875" style="7" customWidth="1"/>
     <col min="5" max="5" width="42" style="7" customWidth="1"/>
     <col min="6" max="6" width="31.44140625" style="2" customWidth="1"/>
-    <col min="7" max="10" width="27.88671875" style="2"/>
-    <col min="11" max="11" width="52.88671875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="40.5546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="27.88671875" style="2"/>
+    <col min="7" max="13" width="27.88671875" style="2"/>
+    <col min="14" max="14" width="52.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="40.5546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="27.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>270</v>
       </c>
@@ -4969,34 +4988,43 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>329</v>
       </c>
@@ -5018,17 +5046,18 @@
       <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="N2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>329</v>
       </c>
@@ -5050,17 +5079,18 @@
       <c r="G3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="H3" s="3"/>
+      <c r="N3" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>329</v>
       </c>
@@ -5082,17 +5112,18 @@
       <c r="G4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="H4" s="3"/>
+      <c r="N4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>329</v>
       </c>
@@ -5114,20 +5145,21 @@
       <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="H5" s="3"/>
+      <c r="N5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>357</v>
       </c>
@@ -5146,20 +5178,21 @@
       <c r="F6" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="3"/>
+      <c r="N6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>329</v>
       </c>
@@ -5181,20 +5214,21 @@
       <c r="G7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="H7" s="3"/>
+      <c r="N7" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>329</v>
       </c>
@@ -5216,20 +5250,21 @@
       <c r="G8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="H8" s="3"/>
+      <c r="N8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>329</v>
       </c>
@@ -5251,17 +5286,18 @@
       <c r="G9" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="H9" s="3"/>
+      <c r="N9" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>329</v>
       </c>
@@ -5283,17 +5319,18 @@
       <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="H10" s="3"/>
+      <c r="N10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>329</v>
       </c>
@@ -5315,17 +5352,18 @@
       <c r="G11" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="H11" s="3"/>
+      <c r="N11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="P11" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
@@ -5347,17 +5385,18 @@
       <c r="G12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="H12" s="3"/>
+      <c r="N12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="P12" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -5379,20 +5418,21 @@
       <c r="G13" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="3"/>
+      <c r="N13" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>353</v>
       </c>
@@ -5414,17 +5454,18 @@
       <c r="G14" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="H14" s="3"/>
+      <c r="N14" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>358</v>
       </c>
@@ -5443,20 +5484,21 @@
       <c r="F15" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="3"/>
+      <c r="N15" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>353</v>
       </c>
@@ -5475,20 +5517,21 @@
       <c r="F16" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="3"/>
+      <c r="N16" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>358</v>
       </c>
@@ -5507,20 +5550,21 @@
       <c r="F17" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="3"/>
+      <c r="N17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
@@ -5542,20 +5586,21 @@
       <c r="G18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="H18" s="3"/>
+      <c r="N18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>358</v>
       </c>
@@ -5574,20 +5619,21 @@
       <c r="F19" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="3"/>
+      <c r="N19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="P19" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>329</v>
       </c>
@@ -5609,17 +5655,18 @@
       <c r="G20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="H20" s="3"/>
+      <c r="N20" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="O20" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="P20" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>360</v>
       </c>
@@ -5641,21 +5688,23 @@
       <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="K21" s="2" t="s">
+      <c r="H21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="N21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="O21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="P21" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="R21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>329</v>
       </c>
@@ -5677,20 +5726,21 @@
       <c r="G22" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="H22" s="3"/>
+      <c r="K22" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="P22" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>329</v>
       </c>
@@ -5712,20 +5762,21 @@
       <c r="G23" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="H23" s="3"/>
+      <c r="N23" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="O23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="R23" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>358</v>
       </c>
@@ -5744,20 +5795,20 @@
       <c r="F24" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>329</v>
       </c>
@@ -5779,17 +5830,18 @@
       <c r="G25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="H25" s="3"/>
+      <c r="N25" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="O25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>360</v>
       </c>
@@ -5808,20 +5860,21 @@
       <c r="F26" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="L26" s="3"/>
+      <c r="N26" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="P26" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>183</v>
       </c>
@@ -5843,17 +5896,18 @@
       <c r="G27" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="H27" s="3"/>
+      <c r="N27" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>193</v>
       </c>
@@ -5875,20 +5929,22 @@
       <c r="G28" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="H28" s="3"/>
+      <c r="K28" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" s="3"/>
+      <c r="N28" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="P28" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>329</v>
       </c>
@@ -5910,17 +5966,18 @@
       <c r="G29" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="H29" s="3"/>
+      <c r="N29" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="P29" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>354</v>
       </c>
@@ -5939,20 +5996,20 @@
       <c r="F30" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="P30" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>362</v>
       </c>
@@ -5974,17 +6031,18 @@
       <c r="G31" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="H31" s="3"/>
+      <c r="N31" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="O31" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="P31" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>329</v>
       </c>
@@ -6003,23 +6061,23 @@
       <c r="F32" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="M32" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>820</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>359</v>
       </c>
@@ -6038,20 +6096,21 @@
       <c r="F33" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="L33" s="3"/>
+      <c r="N33" s="2" t="s">
         <v>821</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="O33" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="P33" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>329</v>
       </c>
@@ -6073,20 +6132,21 @@
       <c r="G34" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="H34" s="3"/>
+      <c r="N34" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="R34" s="2" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>361</v>
       </c>
@@ -6105,20 +6165,21 @@
       <c r="F35" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="K35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="L35" s="3"/>
+      <c r="N35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="O35" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="P35" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>357</v>
       </c>
@@ -6140,21 +6201,23 @@
       <c r="G36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="K36" s="2" t="s">
+      <c r="H36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="N36" s="2" t="s">
         <v>822</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O36" s="2" t="s">
+      <c r="R36" s="2" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>357</v>
       </c>
@@ -6176,23 +6239,25 @@
       <c r="G37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="H37" s="3"/>
+      <c r="K37" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="L37" s="6"/>
+      <c r="N37" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="P37" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="R37" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>360</v>
       </c>
@@ -6214,26 +6279,28 @@
       <c r="G38" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="H38" s="3"/>
+      <c r="K38" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="L38" s="3"/>
+      <c r="M38" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="P38" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="R38" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>362</v>
       </c>
@@ -6255,17 +6322,18 @@
       <c r="G39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="H39" s="3"/>
+      <c r="N39" s="2" t="s">
         <v>823</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>329</v>
       </c>
@@ -6287,17 +6355,18 @@
       <c r="G40" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="H40" s="3"/>
+      <c r="N40" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>358</v>
       </c>
@@ -6319,20 +6388,22 @@
       <c r="G41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="H41" s="3"/>
+      <c r="K41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="L41" s="3"/>
+      <c r="N41" s="2" t="s">
         <v>824</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="P41" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>362</v>
       </c>
@@ -6351,23 +6422,24 @@
       <c r="F42" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="K42" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="J42" s="6" t="s">
+      <c r="L42" s="3"/>
+      <c r="M42" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="P42" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>358</v>
       </c>
@@ -6386,23 +6458,23 @@
       <c r="F43" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="P43" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="44" spans="1:15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>353</v>
       </c>
@@ -6421,21 +6493,23 @@
       <c r="F44" t="s">
         <v>407</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="I44" s="2"/>
-      <c r="K44" t="s">
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="N44" t="s">
         <v>825</v>
       </c>
-      <c r="L44" t="s">
+      <c r="O44" t="s">
         <v>406</v>
       </c>
-      <c r="M44" t="s">
+      <c r="P44" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>329</v>
       </c>
@@ -6454,20 +6528,21 @@
       <c r="F45" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="I45" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="J45" s="3"/>
+      <c r="N45" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="P45" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>360</v>
       </c>
@@ -6486,20 +6561,21 @@
       <c r="F46" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="I46" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="J46" s="3"/>
+      <c r="N46" s="2" t="s">
         <v>826</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="P46" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>329</v>
       </c>
@@ -6521,17 +6597,18 @@
       <c r="G47" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="H47" s="3"/>
+      <c r="N47" s="2" t="s">
         <v>827</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="P47" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>362</v>
       </c>
@@ -6550,20 +6627,21 @@
       <c r="F48" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="I48" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="J48" s="3"/>
+      <c r="N48" s="2" t="s">
         <v>828</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="P48" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>329</v>
       </c>
@@ -6585,20 +6663,21 @@
       <c r="G49" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="H49" s="3"/>
+      <c r="N49" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O49" s="3" t="s">
+      <c r="R49" s="3" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>361</v>
       </c>
@@ -6617,20 +6696,21 @@
       <c r="F50" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="K50" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="3"/>
+      <c r="N50" s="2" t="s">
         <v>829</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="P50" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>329</v>
       </c>
@@ -6652,17 +6732,18 @@
       <c r="G51" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="H51" s="3"/>
+      <c r="N51" s="2" t="s">
         <v>830</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="P51" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>358</v>
       </c>
@@ -6684,26 +6765,29 @@
       <c r="G52" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="3"/>
+      <c r="I52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="J52" s="3"/>
+      <c r="K52" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="3"/>
+      <c r="N52" s="2" t="s">
         <v>831</v>
       </c>
-      <c r="L52" s="2" t="s">
+      <c r="O52" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M52" s="2" t="s">
+      <c r="P52" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O52" s="2" t="s">
+      <c r="R52" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>361</v>
       </c>
@@ -6725,17 +6809,18 @@
       <c r="G53" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="H53" s="3"/>
+      <c r="N53" s="2" t="s">
         <v>832</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="O53" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="M53" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>361</v>
       </c>
@@ -6757,20 +6842,21 @@
       <c r="G54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="H54" s="3"/>
+      <c r="K54" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="N54" s="2" t="s">
         <v>833</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="O54" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="P54" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>362</v>
       </c>
@@ -6789,23 +6875,25 @@
       <c r="F55" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="J55" s="3"/>
+      <c r="K55" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="L55" s="3"/>
+      <c r="N55" s="2" t="s">
         <v>834</v>
       </c>
-      <c r="L55" s="2" t="s">
+      <c r="O55" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="P55" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>353</v>
       </c>
@@ -6824,23 +6912,24 @@
       <c r="F56" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="K56" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="J56" s="3" t="s">
+      <c r="L56" s="3"/>
+      <c r="M56" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>835</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="O56" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="P56" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>361</v>
       </c>
@@ -6859,20 +6948,21 @@
       <c r="F57" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I57" s="3" t="s">
+      <c r="K57" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="K57" s="2" t="s">
+      <c r="L57" s="3"/>
+      <c r="N57" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="L57" s="2" t="s">
+      <c r="O57" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="P57" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>361</v>
       </c>
@@ -6891,17 +6981,18 @@
       <c r="F58" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="K58" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="L58" s="3"/>
+      <c r="N58" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="P58" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>329</v>
       </c>
@@ -6923,17 +7014,18 @@
       <c r="G59" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="H59" s="3"/>
+      <c r="N59" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="O59" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="M59" s="2" t="s">
+      <c r="P59" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>355</v>
       </c>
@@ -6955,20 +7047,21 @@
       <c r="G60" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="H60" s="3"/>
+      <c r="K60" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="N60" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="O60" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="P60" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>329</v>
       </c>
@@ -6987,20 +7080,21 @@
       <c r="F61" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="K61" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="3"/>
+      <c r="N61" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L61" s="2" t="s">
+      <c r="O61" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M61" s="2" t="s">
+      <c r="P61" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>360</v>
       </c>
@@ -7019,23 +7113,24 @@
       <c r="F62" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="K62" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="L62" s="3"/>
+      <c r="M62" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="L62" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="M62" s="2" t="s">
+      <c r="P62" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>358</v>
       </c>
@@ -7054,23 +7149,24 @@
       <c r="F63" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="K63" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="K63" s="2" t="s">
+      <c r="L63" s="3"/>
+      <c r="N63" s="2" t="s">
         <v>837</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="O63" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="M63" s="2" t="s">
+      <c r="P63" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O63" s="2" t="s">
+      <c r="R63" s="2" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>329</v>
       </c>
@@ -7092,23 +7188,25 @@
       <c r="G64" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="H64" s="3"/>
+      <c r="K64" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="L64" s="3"/>
+      <c r="M64" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="N64" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="O64" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="M64" s="2" t="s">
+      <c r="P64" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>356</v>
       </c>
@@ -7130,23 +7228,25 @@
       <c r="G65" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="H65" s="3"/>
+      <c r="K65" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="L65" s="3"/>
+      <c r="M65" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="N65" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="O65" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="P65" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>360</v>
       </c>
@@ -7168,17 +7268,18 @@
       <c r="G66" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="H66" s="3"/>
+      <c r="N66" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="L66" s="2" t="s">
+      <c r="O66" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="M66" s="2" t="s">
+      <c r="P66" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>353</v>
       </c>
@@ -7197,23 +7298,24 @@
       <c r="F67" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="K67" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="J67" s="3" t="s">
+      <c r="L67" s="3"/>
+      <c r="M67" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="K67" s="2" t="s">
+      <c r="N67" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="O67" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="M67" s="2" t="s">
+      <c r="P67" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>360</v>
       </c>
@@ -7232,23 +7334,24 @@
       <c r="F68" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="K68" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="J68" s="3" t="s">
+      <c r="L68" s="3"/>
+      <c r="M68" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="N68" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="O68" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="M68" s="2" t="s">
+      <c r="P68" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>329</v>
       </c>
@@ -7270,20 +7373,22 @@
       <c r="G69" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" s="3"/>
+      <c r="I69" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="J69" s="3"/>
+      <c r="N69" s="2" t="s">
         <v>840</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="O69" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="M69" s="2" t="s">
+      <c r="P69" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>362</v>
       </c>
@@ -7302,23 +7407,24 @@
       <c r="F70" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="K70" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="L70" s="3"/>
+      <c r="M70" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="N70" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="O70" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="M70" s="2" t="s">
+      <c r="P70" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>358</v>
       </c>
@@ -7337,23 +7443,24 @@
       <c r="F71" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I71" s="3" t="s">
+      <c r="K71" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J71" s="3" t="s">
+      <c r="L71" s="3"/>
+      <c r="M71" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="K71" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="O71" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="M71" s="2" t="s">
+      <c r="P71" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>361</v>
       </c>
@@ -7375,23 +7482,25 @@
       <c r="G72" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="H72" s="3"/>
+      <c r="K72" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="L72" s="3"/>
+      <c r="N72" s="2" t="s">
         <v>841</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="O72" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M72" s="2" t="s">
+      <c r="P72" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="O72" s="2" t="s">
+      <c r="R72" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>361</v>
       </c>
@@ -7410,20 +7519,21 @@
       <c r="F73" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="K73" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="3"/>
+      <c r="N73" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="O73" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="P73" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>329</v>
       </c>
@@ -7442,23 +7552,24 @@
       <c r="F74" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="K74" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="J74" s="3" t="s">
+      <c r="L74" s="3"/>
+      <c r="M74" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="N74" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L74" s="2" t="s">
+      <c r="O74" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="P74" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>362</v>
       </c>
@@ -7477,20 +7588,21 @@
       <c r="F75" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="K75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="L75" s="3"/>
+      <c r="N75" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="O75" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="P75" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>361</v>
       </c>
@@ -7512,23 +7624,25 @@
       <c r="G76" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I76" s="3" t="s">
+      <c r="H76" s="3"/>
+      <c r="K76" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J76" s="2" t="s">
+      <c r="L76" s="3"/>
+      <c r="M76" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="N76" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="O76" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="M76" s="2" t="s">
+      <c r="P76" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>329</v>
       </c>
@@ -7550,23 +7664,24 @@
       <c r="G77" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="H77" s="3"/>
+      <c r="K77" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J77" s="3" t="s">
+      <c r="M77" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="N77" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="O77" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="M77" s="2" t="s">
+      <c r="P77" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>355</v>
       </c>
@@ -7585,23 +7700,24 @@
       <c r="F78" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I78" s="3" t="s">
+      <c r="K78" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J78" s="3" t="s">
+      <c r="L78" s="3"/>
+      <c r="M78" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="N78" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="O78" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="P78" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>40</v>
       </c>
@@ -7620,20 +7736,21 @@
       <c r="F79" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I79" s="3" t="s">
+      <c r="K79" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="L79" s="3"/>
+      <c r="N79" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="O79" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="P79" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>329</v>
       </c>
@@ -7652,23 +7769,24 @@
       <c r="F80" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="I80" s="3" t="s">
+      <c r="K80" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="3"/>
+      <c r="N80" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="O80" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="P80" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O80" s="2" t="s">
+      <c r="R80" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>360</v>
       </c>
@@ -7690,23 +7808,25 @@
       <c r="G81" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I81" s="3" t="s">
+      <c r="H81" s="3"/>
+      <c r="K81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J81" s="2" t="s">
+      <c r="L81" s="3"/>
+      <c r="M81" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="K81" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="L81" s="2" t="s">
+      <c r="O81" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="P81" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>352</v>
       </c>
@@ -7728,20 +7848,22 @@
       <c r="G82" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I82" s="3" t="s">
+      <c r="H82" s="3"/>
+      <c r="K82" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="L82" s="3"/>
+      <c r="N82" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="L82" s="2" t="s">
+      <c r="O82" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="P82" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>329</v>
       </c>
@@ -7760,20 +7882,21 @@
       <c r="F83" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I83" s="3" t="s">
+      <c r="K83" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="L83" s="3"/>
+      <c r="N83" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="L83" s="2" t="s">
+      <c r="O83" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="P83" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>353</v>
       </c>
@@ -7795,23 +7918,25 @@
       <c r="G84" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H84" s="3"/>
+      <c r="I84" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="J84" s="3"/>
+      <c r="N84" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="L84" s="2" t="s">
+      <c r="O84" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="M84" s="2" t="s">
+      <c r="P84" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="O84" s="2" t="s">
+      <c r="R84" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>360</v>
       </c>
@@ -7830,20 +7955,21 @@
       <c r="F85" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="K85" s="2" t="s">
+      <c r="J85" s="3"/>
+      <c r="N85" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="L85" s="2" t="s">
+      <c r="O85" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="M85" s="2" t="s">
+      <c r="P85" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>353</v>
       </c>
@@ -7862,20 +7988,21 @@
       <c r="F86" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I86" s="3" t="s">
+      <c r="K86" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="L86" s="3"/>
+      <c r="N86" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="L86" s="2" t="s">
+      <c r="O86" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="M86" s="2" t="s">
+      <c r="P86" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>360</v>
       </c>
@@ -7894,23 +8021,24 @@
       <c r="F87" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I87" s="3" t="s">
+      <c r="K87" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J87" s="3" t="s">
+      <c r="L87" s="3"/>
+      <c r="M87" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="K87" s="2" t="s">
+      <c r="N87" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="L87" s="2" t="s">
+      <c r="O87" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="M87" s="2" t="s">
+      <c r="P87" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>361</v>
       </c>
@@ -7929,23 +8057,24 @@
       <c r="F88" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I88" s="3" t="s">
+      <c r="K88" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="J88" s="3" t="s">
+      <c r="L88" s="3"/>
+      <c r="M88" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="N88" s="2" t="s">
         <v>845</v>
       </c>
-      <c r="L88" s="2" t="s">
+      <c r="O88" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="M88" s="2" t="s">
+      <c r="P88" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>353</v>
       </c>
@@ -7964,23 +8093,24 @@
       <c r="F89" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I89" s="3" t="s">
+      <c r="K89" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="J89" s="3" t="s">
+      <c r="L89" s="3"/>
+      <c r="M89" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="K89" s="2" t="s">
+      <c r="N89" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="L89" s="2" t="s">
+      <c r="O89" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="M89" s="2" t="s">
+      <c r="P89" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>358</v>
       </c>
@@ -8002,17 +8132,18 @@
       <c r="G90" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="K90" s="2" t="s">
+      <c r="H90" s="3"/>
+      <c r="N90" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="L90" s="2" t="s">
+      <c r="O90" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M90" s="2" t="s">
+      <c r="P90" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>329</v>
       </c>
@@ -8034,26 +8165,29 @@
       <c r="G91" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="H91" s="3"/>
+      <c r="I91" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="I91" s="3" t="s">
+      <c r="J91" s="3"/>
+      <c r="K91" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="J91" s="3" t="s">
+      <c r="L91" s="3"/>
+      <c r="M91" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="K91" s="2" t="s">
+      <c r="N91" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="L91" s="2" t="s">
+      <c r="O91" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="M91" s="2" t="s">
+      <c r="P91" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>353</v>
       </c>
@@ -8072,23 +8206,24 @@
       <c r="F92" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="K92" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="J92" s="3" t="s">
+      <c r="L92" s="3"/>
+      <c r="M92" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="K92" s="2" t="s">
+      <c r="N92" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="L92" s="2" t="s">
+      <c r="O92" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="M92" s="2" t="s">
+      <c r="P92" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>358</v>
       </c>
@@ -8110,20 +8245,22 @@
       <c r="G93" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="H93" s="3"/>
+      <c r="K93" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="K93" s="2" t="s">
+      <c r="L93" s="3"/>
+      <c r="N93" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="L93" s="2" t="s">
+      <c r="O93" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="M93" s="2" t="s">
+      <c r="P93" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>355</v>
       </c>
@@ -8142,20 +8279,21 @@
       <c r="F94" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="K94" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="K94" s="2" t="s">
+      <c r="L94" s="3"/>
+      <c r="N94" s="2" t="s">
         <v>846</v>
       </c>
-      <c r="L94" s="2" t="s">
+      <c r="O94" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="M94" s="2" t="s">
+      <c r="P94" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>360</v>
       </c>
@@ -8174,20 +8312,21 @@
       <c r="F95" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="I95" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="K95" s="2" t="s">
+      <c r="J95" s="3"/>
+      <c r="N95" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="L95" s="2" t="s">
+      <c r="O95" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="M95" s="2" t="s">
+      <c r="P95" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>358</v>
       </c>
@@ -8206,20 +8345,20 @@
       <c r="F96" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="K96" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="K96" s="2" t="s">
+      <c r="N96" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="L96" s="2" t="s">
+      <c r="O96" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="M96" s="2" t="s">
+      <c r="P96" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>360</v>
       </c>
@@ -8238,20 +8377,20 @@
       <c r="F97" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="K97" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="K97" s="2" t="s">
+      <c r="N97" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="L97" s="2" t="s">
+      <c r="O97" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="M97" s="2" t="s">
+      <c r="P97" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>329</v>
       </c>
@@ -8270,20 +8409,20 @@
       <c r="F98" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="K98" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="K98" s="2" t="s">
+      <c r="N98" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="L98" s="2" t="s">
+      <c r="O98" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="M98" s="2" t="s">
+      <c r="P98" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>40</v>
       </c>
@@ -8302,20 +8441,20 @@
       <c r="F99" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="K99" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="K99" s="10" t="s">
+      <c r="N99" s="10" t="s">
         <v>661</v>
       </c>
-      <c r="L99" s="2" t="s">
+      <c r="O99" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="M99" s="2" t="s">
+      <c r="P99" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>358</v>
       </c>
@@ -8334,20 +8473,20 @@
       <c r="F100" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="H100" s="2" t="s">
+      <c r="I100" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="K100" s="2" t="s">
+      <c r="N100" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="L100" s="2" t="s">
+      <c r="O100" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="M100" s="2" t="s">
+      <c r="P100" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>358</v>
       </c>
@@ -8366,20 +8505,20 @@
       <c r="F101" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="K101" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="K101" s="2" t="s">
+      <c r="N101" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="L101" s="2" t="s">
+      <c r="O101" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="M101" s="2" t="s">
+      <c r="P101" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>329</v>
       </c>
@@ -8398,20 +8537,20 @@
       <c r="F102" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="K102" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="K102" s="2" t="s">
+      <c r="N102" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="L102" s="2" t="s">
+      <c r="O102" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="M102" s="2" t="s">
+      <c r="P102" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>40</v>
       </c>
@@ -8430,20 +8569,20 @@
       <c r="F103" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="K103" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="K103" s="2" t="s">
+      <c r="N103" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="L103" s="2" t="s">
+      <c r="O103" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="M103" s="2" t="s">
+      <c r="P103" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>329</v>
       </c>
@@ -8465,17 +8604,17 @@
       <c r="G104" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="K104" s="2" t="s">
+      <c r="N104" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="L104" s="2" t="s">
+      <c r="O104" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="M104" s="2" t="s">
+      <c r="P104" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>329</v>
       </c>
@@ -8494,20 +8633,20 @@
       <c r="F105" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="K105" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="K105" s="2" t="s">
+      <c r="N105" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="L105" s="2" t="s">
+      <c r="O105" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="M105" s="2" t="s">
+      <c r="P105" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>329</v>
       </c>
@@ -8529,17 +8668,17 @@
       <c r="G106" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="K106" s="2" t="s">
+      <c r="N106" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="L106" s="2" t="s">
+      <c r="O106" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="M106" s="2" t="s">
+      <c r="P106" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>360</v>
       </c>
@@ -8558,20 +8697,20 @@
       <c r="F107" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="K107" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="K107" s="2" t="s">
+      <c r="N107" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="L107" s="2" t="s">
+      <c r="O107" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="M107" s="2" t="s">
+      <c r="P107" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>329</v>
       </c>
@@ -8593,17 +8732,17 @@
       <c r="G108" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="K108" s="10" t="s">
+      <c r="N108" s="10" t="s">
         <v>670</v>
       </c>
-      <c r="L108" s="2" t="s">
+      <c r="O108" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="M108" s="2" t="s">
+      <c r="P108" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>353</v>
       </c>
@@ -8622,20 +8761,20 @@
       <c r="F109" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I109" s="2" t="s">
+      <c r="K109" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="K109" s="2" t="s">
+      <c r="N109" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="L109" s="2" t="s">
+      <c r="O109" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="M109" s="2" t="s">
+      <c r="P109" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>329</v>
       </c>
@@ -8657,17 +8796,17 @@
       <c r="G110" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="K110" s="2" t="s">
+      <c r="N110" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="L110" s="2" t="s">
+      <c r="O110" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="M110" s="2" t="s">
+      <c r="P110" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>40</v>
       </c>
@@ -8686,20 +8825,20 @@
       <c r="F111" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="I111" s="2" t="s">
+      <c r="K111" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="K111" s="2" t="s">
+      <c r="N111" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="L111" s="2" t="s">
+      <c r="O111" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="M111" s="2" t="s">
+      <c r="P111" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>360</v>
       </c>
@@ -8718,20 +8857,20 @@
       <c r="F112" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="K112" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="K112" s="2" t="s">
+      <c r="N112" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="L112" s="2" t="s">
+      <c r="O112" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="M112" s="2" t="s">
+      <c r="P112" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>329</v>
       </c>
@@ -8753,17 +8892,18 @@
       <c r="G113" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="K113" s="2" t="s">
+      <c r="H113" s="3"/>
+      <c r="N113" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="L113" s="2" t="s">
+      <c r="O113" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="M113" s="2" t="s">
+      <c r="P113" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>40</v>
       </c>
@@ -8785,17 +8925,18 @@
       <c r="G114" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="K114" s="2" t="s">
+      <c r="H114" s="3"/>
+      <c r="N114" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="L114" s="2" t="s">
+      <c r="O114" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="M114" s="2" t="s">
+      <c r="P114" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="115" spans="1:13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>329</v>
       </c>
@@ -8814,21 +8955,22 @@
       <c r="F115" t="s">
         <v>541</v>
       </c>
-      <c r="H115" s="2"/>
-      <c r="I115" t="s">
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" t="s">
         <v>745</v>
       </c>
-      <c r="K115" t="s">
+      <c r="N115" t="s">
         <v>855</v>
       </c>
-      <c r="L115" t="s">
+      <c r="O115" t="s">
         <v>808</v>
       </c>
-      <c r="M115" t="s">
+      <c r="P115" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="116" spans="1:13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>329</v>
       </c>
@@ -8847,22 +8989,24 @@
       <c r="F116" t="s">
         <v>528</v>
       </c>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2" t="s">
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="J116" s="2"/>
-      <c r="K116" t="s">
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" t="s">
         <v>749</v>
       </c>
-      <c r="L116" t="s">
+      <c r="O116" t="s">
         <v>809</v>
       </c>
-      <c r="M116" t="s">
+      <c r="P116" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="117" spans="1:13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>329</v>
       </c>
@@ -8881,22 +9025,24 @@
       <c r="F117" t="s">
         <v>620</v>
       </c>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2" t="s">
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="J117" s="2"/>
-      <c r="K117" t="s">
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" t="s">
         <v>750</v>
       </c>
-      <c r="L117" t="s">
+      <c r="O117" t="s">
         <v>810</v>
       </c>
-      <c r="M117" t="s">
+      <c r="P117" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>329</v>
       </c>
@@ -8915,20 +9061,20 @@
       <c r="F118" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="K118" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="K118" s="2" t="s">
+      <c r="N118" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="O118" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="M118" s="2" t="s">
+      <c r="P118" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>329</v>
       </c>
@@ -8947,20 +9093,20 @@
       <c r="F119" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="K119" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="K119" s="2" t="s">
+      <c r="N119" s="2" t="s">
         <v>854</v>
       </c>
-      <c r="L119" s="2" t="s">
+      <c r="O119" s="2" t="s">
         <v>812</v>
       </c>
-      <c r="M119" s="2" t="s">
+      <c r="P119" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>360</v>
       </c>
@@ -8979,20 +9125,20 @@
       <c r="F120" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I120" s="2" t="s">
+      <c r="K120" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="K120" s="2" t="s">
+      <c r="N120" s="2" t="s">
         <v>853</v>
       </c>
-      <c r="L120" s="2" t="s">
+      <c r="O120" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="M120" s="2" t="s">
+      <c r="P120" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>360</v>
       </c>
@@ -9011,20 +9157,21 @@
       <c r="F121" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I121" s="3" t="s">
+      <c r="K121" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="K121" s="2" t="s">
+      <c r="L121" s="3"/>
+      <c r="N121" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="L121" s="2" t="s">
+      <c r="O121" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="M121" s="2" t="s">
+      <c r="P121" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>329</v>
       </c>
@@ -9043,20 +9190,21 @@
       <c r="F122" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I122" s="3" t="s">
+      <c r="K122" s="3" t="s">
         <v>767</v>
       </c>
-      <c r="K122" s="2" t="s">
+      <c r="L122" s="3"/>
+      <c r="N122" s="2" t="s">
         <v>851</v>
       </c>
-      <c r="L122" s="2" t="s">
+      <c r="O122" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="M122" s="2" t="s">
+      <c r="P122" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>40</v>
       </c>
@@ -9075,20 +9223,21 @@
       <c r="F123" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I123" s="3" t="s">
+      <c r="K123" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="K123" s="2" t="s">
+      <c r="L123" s="3"/>
+      <c r="N123" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="L123" s="2" t="s">
+      <c r="O123" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="M123" s="2" t="s">
+      <c r="P123" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>358</v>
       </c>
@@ -9107,20 +9256,21 @@
       <c r="F124" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I124" s="3" t="s">
+      <c r="K124" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="K124" s="2" t="s">
+      <c r="L124" s="3"/>
+      <c r="N124" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="L124" s="2" t="s">
+      <c r="O124" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="M124" s="2" t="s">
+      <c r="P124" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>329</v>
       </c>
@@ -9142,17 +9292,18 @@
       <c r="G125" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="K125" s="2" t="s">
+      <c r="H125" s="3"/>
+      <c r="N125" s="2" t="s">
         <v>850</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="O125" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="M125" s="2" t="s">
+      <c r="P125" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>360</v>
       </c>
@@ -9171,20 +9322,21 @@
       <c r="F126" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I126" s="3" t="s">
+      <c r="K126" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="K126" s="2" t="s">
+      <c r="L126" s="3"/>
+      <c r="N126" s="2" t="s">
         <v>849</v>
       </c>
-      <c r="L126" s="2" t="s">
+      <c r="O126" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="M126" s="2" t="s">
+      <c r="P126" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>358</v>
       </c>
@@ -9203,20 +9355,21 @@
       <c r="F127" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="I127" s="3" t="s">
+      <c r="K127" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="K127" s="2" t="s">
+      <c r="L127" s="3"/>
+      <c r="N127" s="2" t="s">
         <v>848</v>
       </c>
-      <c r="L127" s="2" t="s">
+      <c r="O127" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="M127" s="2" t="s">
+      <c r="P127" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>329</v>
       </c>
@@ -9235,22 +9388,49 @@
       <c r="F128" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="I128" s="3" t="s">
+      <c r="K128" s="3" t="s">
         <v>790</v>
       </c>
-      <c r="K128" s="2" t="s">
+      <c r="L128" s="3"/>
+      <c r="N128" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="L128" s="2" t="s">
+      <c r="O128" s="2" t="s">
         <v>817</v>
       </c>
-      <c r="M128" s="2" t="s">
+      <c r="P128" s="2" t="s">
         <v>376</v>
       </c>
     </row>
+    <row r="129" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B129" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="N129" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="O129" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="P129" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O114" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O96">
+  <autoFilter ref="A1:R114" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R96">
       <sortCondition ref="B1:B53"/>
     </sortState>
   </autoFilter>
@@ -9266,56 +9446,56 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G52" r:id="rId1" xr:uid="{F3A125A7-06CF-46C5-AF31-507DA2383A6C}"/>
-    <hyperlink ref="I15" r:id="rId2" xr:uid="{E7EF4AE3-28CB-47CB-9919-7AFD9088563B}"/>
-    <hyperlink ref="I16" r:id="rId3" xr:uid="{76D249F5-5556-4F11-989E-7D5C5CDD47EC}"/>
-    <hyperlink ref="I26" r:id="rId4" xr:uid="{9B78C140-3576-4D09-95BD-EAD3E62448DC}"/>
-    <hyperlink ref="I37" r:id="rId5" xr:uid="{99B560E0-9392-4F6A-B5FD-4FD74293E06B}"/>
+    <hyperlink ref="K15" r:id="rId2" xr:uid="{E7EF4AE3-28CB-47CB-9919-7AFD9088563B}"/>
+    <hyperlink ref="K16" r:id="rId3" xr:uid="{76D249F5-5556-4F11-989E-7D5C5CDD47EC}"/>
+    <hyperlink ref="K26" r:id="rId4" xr:uid="{9B78C140-3576-4D09-95BD-EAD3E62448DC}"/>
+    <hyperlink ref="K37" r:id="rId5" xr:uid="{99B560E0-9392-4F6A-B5FD-4FD74293E06B}"/>
     <hyperlink ref="G47" r:id="rId6" xr:uid="{C26B23F8-6AFC-41BF-849A-BBA58B0795CF}"/>
     <hyperlink ref="G66" r:id="rId7" xr:uid="{7380E165-8C1D-4C54-A16B-E5C2E6A02DD4}"/>
-    <hyperlink ref="I28" r:id="rId8" xr:uid="{F77926D1-456A-48C5-80A4-2B9DF5FAF089}"/>
+    <hyperlink ref="K28" r:id="rId8" xr:uid="{F77926D1-456A-48C5-80A4-2B9DF5FAF089}"/>
     <hyperlink ref="G29" r:id="rId9" xr:uid="{2DC49B32-9D5A-42DF-BF50-C99DA3DC9750}"/>
-    <hyperlink ref="I62" r:id="rId10" xr:uid="{1A440453-6034-4CEF-B7E6-33B3E7A76D24}"/>
-    <hyperlink ref="I88" r:id="rId11" xr:uid="{C1DBFCF3-2571-4AE1-AE01-01B95EE31641}"/>
-    <hyperlink ref="J88" r:id="rId12" xr:uid="{D9EB99F0-1F8C-4011-B4D1-964F97B5BF75}"/>
-    <hyperlink ref="I89" r:id="rId13" xr:uid="{8D720BD3-9B2F-4D56-938E-C74C72815243}"/>
-    <hyperlink ref="I68" r:id="rId14" xr:uid="{9B42E3B3-2B0D-44B1-80CF-8CADAD4DB5BE}"/>
-    <hyperlink ref="J91" r:id="rId15" xr:uid="{7D1C4D84-F3A9-4ACE-9988-5FFD199B7021}"/>
-    <hyperlink ref="I92" r:id="rId16" xr:uid="{CF040F9F-5A9A-43B5-99F3-769106AE345D}"/>
-    <hyperlink ref="J92" r:id="rId17" xr:uid="{6946CAEC-DD7D-4E78-A567-1F8291BCE01F}"/>
+    <hyperlink ref="K62" r:id="rId10" xr:uid="{1A440453-6034-4CEF-B7E6-33B3E7A76D24}"/>
+    <hyperlink ref="K88" r:id="rId11" xr:uid="{C1DBFCF3-2571-4AE1-AE01-01B95EE31641}"/>
+    <hyperlink ref="M88" r:id="rId12" xr:uid="{D9EB99F0-1F8C-4011-B4D1-964F97B5BF75}"/>
+    <hyperlink ref="K89" r:id="rId13" xr:uid="{8D720BD3-9B2F-4D56-938E-C74C72815243}"/>
+    <hyperlink ref="K68" r:id="rId14" xr:uid="{9B42E3B3-2B0D-44B1-80CF-8CADAD4DB5BE}"/>
+    <hyperlink ref="M91" r:id="rId15" xr:uid="{7D1C4D84-F3A9-4ACE-9988-5FFD199B7021}"/>
+    <hyperlink ref="K92" r:id="rId16" xr:uid="{CF040F9F-5A9A-43B5-99F3-769106AE345D}"/>
+    <hyperlink ref="M92" r:id="rId17" xr:uid="{6946CAEC-DD7D-4E78-A567-1F8291BCE01F}"/>
     <hyperlink ref="G84" r:id="rId18" xr:uid="{0333C02F-316B-4FAF-ABF2-B31D63CEA970}"/>
-    <hyperlink ref="I56" r:id="rId19" xr:uid="{C70585B8-DB5D-41B9-A8EA-6ABAA31CEE25}"/>
-    <hyperlink ref="J56" r:id="rId20" xr:uid="{3F49FD62-E57F-4893-99D8-D17515A177D4}"/>
-    <hyperlink ref="I93" r:id="rId21" xr:uid="{ADAD267C-8EBD-4962-AC91-D7411BC2CE77}"/>
+    <hyperlink ref="K56" r:id="rId19" xr:uid="{C70585B8-DB5D-41B9-A8EA-6ABAA31CEE25}"/>
+    <hyperlink ref="M56" r:id="rId20" xr:uid="{3F49FD62-E57F-4893-99D8-D17515A177D4}"/>
+    <hyperlink ref="K93" r:id="rId21" xr:uid="{ADAD267C-8EBD-4962-AC91-D7411BC2CE77}"/>
     <hyperlink ref="G93" r:id="rId22" xr:uid="{53DC4FF4-9BDC-4B12-B134-DCFF8CF9A0B6}"/>
     <hyperlink ref="G69" r:id="rId23" xr:uid="{D411639D-B795-495E-AFF8-9E75B3104B2E}"/>
-    <hyperlink ref="H69" r:id="rId24" xr:uid="{D2E3041F-136B-406C-AEFD-ECD5DDCCEE8D}"/>
-    <hyperlink ref="I86" r:id="rId25" xr:uid="{36F20F9B-87FD-43F3-AA82-998C317E87A0}"/>
+    <hyperlink ref="I69" r:id="rId24" xr:uid="{D2E3041F-136B-406C-AEFD-ECD5DDCCEE8D}"/>
+    <hyperlink ref="K86" r:id="rId25" xr:uid="{36F20F9B-87FD-43F3-AA82-998C317E87A0}"/>
     <hyperlink ref="G49" r:id="rId26" xr:uid="{FE6EA451-7373-4673-B26F-8064A68D4B4C}"/>
-    <hyperlink ref="I70" r:id="rId27" xr:uid="{D85D8F0D-80FB-462B-979F-96969B609670}"/>
-    <hyperlink ref="I94" r:id="rId28" xr:uid="{9657BD2F-C84D-4FEB-A4C4-2D26D95999AC}"/>
+    <hyperlink ref="K70" r:id="rId27" xr:uid="{D85D8F0D-80FB-462B-979F-96969B609670}"/>
+    <hyperlink ref="K94" r:id="rId28" xr:uid="{9657BD2F-C84D-4FEB-A4C4-2D26D95999AC}"/>
     <hyperlink ref="G31" r:id="rId29" xr:uid="{A3AF382D-9F1F-438A-8587-CD3F0E5C4E0C}"/>
-    <hyperlink ref="H52" r:id="rId30" xr:uid="{5A357219-4CCF-4FF8-9FBA-7BC83C8AA05D}"/>
-    <hyperlink ref="I33" r:id="rId31" xr:uid="{68E034BC-CFF4-47C0-AFAD-7BA9EA99E824}"/>
-    <hyperlink ref="I50" r:id="rId32" xr:uid="{A23C2C5B-A202-448D-AE34-DDD1EFFA348F}"/>
-    <hyperlink ref="I57" r:id="rId33" xr:uid="{AB970F8D-FF1E-49FE-B9C1-9D49470D1F60}"/>
-    <hyperlink ref="I72" r:id="rId34" xr:uid="{8808B1A0-81D2-4098-983B-5BFD59F874B5}"/>
-    <hyperlink ref="I71" r:id="rId35" xr:uid="{BF156D20-C0B1-47EF-8AC8-7F08C279366F}"/>
-    <hyperlink ref="H95" r:id="rId36" xr:uid="{99DF1605-5944-41A6-AED4-A518CB472F3B}"/>
-    <hyperlink ref="O49" r:id="rId37" display="https://www.jasp-online.org/asjournal/summer-2019/designs-of-experiments-doe-in-survivability-testing/" xr:uid="{3D4C927E-73EB-4E83-8788-3EB47DDD1C73}"/>
+    <hyperlink ref="I52" r:id="rId30" xr:uid="{5A357219-4CCF-4FF8-9FBA-7BC83C8AA05D}"/>
+    <hyperlink ref="K33" r:id="rId31" xr:uid="{68E034BC-CFF4-47C0-AFAD-7BA9EA99E824}"/>
+    <hyperlink ref="K50" r:id="rId32" xr:uid="{A23C2C5B-A202-448D-AE34-DDD1EFFA348F}"/>
+    <hyperlink ref="K57" r:id="rId33" xr:uid="{AB970F8D-FF1E-49FE-B9C1-9D49470D1F60}"/>
+    <hyperlink ref="K72" r:id="rId34" xr:uid="{8808B1A0-81D2-4098-983B-5BFD59F874B5}"/>
+    <hyperlink ref="K71" r:id="rId35" xr:uid="{BF156D20-C0B1-47EF-8AC8-7F08C279366F}"/>
+    <hyperlink ref="I95" r:id="rId36" xr:uid="{99DF1605-5944-41A6-AED4-A518CB472F3B}"/>
+    <hyperlink ref="R49" r:id="rId37" display="https://www.jasp-online.org/asjournal/summer-2019/designs-of-experiments-doe-in-survivability-testing/" xr:uid="{3D4C927E-73EB-4E83-8788-3EB47DDD1C73}"/>
     <hyperlink ref="G54" r:id="rId38" xr:uid="{C35B1FD4-DC5F-4516-BC64-619A82141111}"/>
     <hyperlink ref="G2" r:id="rId39" xr:uid="{B775C6CE-21D0-47A4-A2AB-58A5C36A85AE}"/>
-    <hyperlink ref="J38" r:id="rId40" xr:uid="{7476C431-6029-4DF1-87BD-7959CD9C0A17}"/>
-    <hyperlink ref="J64" r:id="rId41" xr:uid="{A7D75B17-314C-43E9-9131-3E28D8BF54EE}"/>
-    <hyperlink ref="J74" r:id="rId42" xr:uid="{8AB4A742-D3D7-48EF-86C6-0125D9B6499A}"/>
-    <hyperlink ref="J77" r:id="rId43" xr:uid="{149333D5-9EA5-4902-977E-C2D501E057FD}"/>
-    <hyperlink ref="J87" r:id="rId44" xr:uid="{1F62F507-6791-442E-B20F-9134DCD4FED0}"/>
-    <hyperlink ref="J89" r:id="rId45" xr:uid="{64C6046A-C792-406B-8B6C-8DCAF3048A3B}"/>
-    <hyperlink ref="J67" r:id="rId46" xr:uid="{C3CBAA9C-35D3-491F-A376-7BE070E1FB3E}"/>
-    <hyperlink ref="J78" r:id="rId47" xr:uid="{1BE6E912-6E7A-4367-87E1-D064F76D813F}"/>
+    <hyperlink ref="M38" r:id="rId40" xr:uid="{7476C431-6029-4DF1-87BD-7959CD9C0A17}"/>
+    <hyperlink ref="M64" r:id="rId41" xr:uid="{A7D75B17-314C-43E9-9131-3E28D8BF54EE}"/>
+    <hyperlink ref="M74" r:id="rId42" xr:uid="{8AB4A742-D3D7-48EF-86C6-0125D9B6499A}"/>
+    <hyperlink ref="M77" r:id="rId43" xr:uid="{149333D5-9EA5-4902-977E-C2D501E057FD}"/>
+    <hyperlink ref="M87" r:id="rId44" xr:uid="{1F62F507-6791-442E-B20F-9134DCD4FED0}"/>
+    <hyperlink ref="M89" r:id="rId45" xr:uid="{64C6046A-C792-406B-8B6C-8DCAF3048A3B}"/>
+    <hyperlink ref="M67" r:id="rId46" xr:uid="{C3CBAA9C-35D3-491F-A376-7BE070E1FB3E}"/>
+    <hyperlink ref="M78" r:id="rId47" xr:uid="{1BE6E912-6E7A-4367-87E1-D064F76D813F}"/>
     <hyperlink ref="G3" r:id="rId48" xr:uid="{ED582C3E-6316-4B94-B4F5-6747C01E88E6}"/>
     <hyperlink ref="G4" r:id="rId49" xr:uid="{6072E6A5-23E9-41F9-BF45-992C15F9823A}"/>
     <hyperlink ref="G5" r:id="rId50" xr:uid="{77A8F22A-3F65-41C0-86B0-36BFA2D0BD86}"/>
-    <hyperlink ref="I6" r:id="rId51" xr:uid="{9F780E94-F373-41D2-86DA-9C9A6B2E2498}"/>
+    <hyperlink ref="K6" r:id="rId51" xr:uid="{9F780E94-F373-41D2-86DA-9C9A6B2E2498}"/>
     <hyperlink ref="G7" r:id="rId52" xr:uid="{A338A5F1-473E-47A2-8629-BF867FB7695E}"/>
     <hyperlink ref="G8" r:id="rId53" xr:uid="{570688FA-B859-4A6F-8231-0137946CACCF}"/>
     <hyperlink ref="G9" r:id="rId54" xr:uid="{2C045606-DE0A-48F0-8949-424FAE793FC5}"/>
@@ -9323,10 +9503,10 @@
     <hyperlink ref="G11" r:id="rId56" xr:uid="{72ADE713-705B-4167-AF73-DF0176A84AE2}"/>
     <hyperlink ref="G12" r:id="rId57" xr:uid="{728DF1EA-75F6-4A19-80A6-7F1FA430E774}"/>
     <hyperlink ref="G14" r:id="rId58" xr:uid="{5836CF11-C32B-44A4-A7B8-E4D372FAE973}"/>
-    <hyperlink ref="I13" r:id="rId59" xr:uid="{98B0DF65-6891-4395-8A17-7DB1689BF624}"/>
-    <hyperlink ref="I17" r:id="rId60" xr:uid="{2CF7558A-A9C5-479B-9EAF-F08A63292CC3}"/>
+    <hyperlink ref="K13" r:id="rId59" xr:uid="{98B0DF65-6891-4395-8A17-7DB1689BF624}"/>
+    <hyperlink ref="K17" r:id="rId60" xr:uid="{2CF7558A-A9C5-479B-9EAF-F08A63292CC3}"/>
     <hyperlink ref="G18" r:id="rId61" xr:uid="{C8F9B671-E662-4D89-AA2F-7D617004443A}"/>
-    <hyperlink ref="I19" r:id="rId62" xr:uid="{1C832169-66C7-4C45-8699-A6F23F3A28E5}"/>
+    <hyperlink ref="K19" r:id="rId62" xr:uid="{1C832169-66C7-4C45-8699-A6F23F3A28E5}"/>
     <hyperlink ref="G20" r:id="rId63" xr:uid="{BF11C286-EADD-4301-9917-683B5897E3FB}"/>
     <hyperlink ref="G21" r:id="rId64" xr:uid="{F59906C8-9DE8-456D-8586-B615F5C13EAD}"/>
     <hyperlink ref="G22" r:id="rId65" xr:uid="{D45FC2C8-C6C2-4CFC-A726-582CEAC84585}"/>
@@ -9334,60 +9514,60 @@
     <hyperlink ref="G25" r:id="rId67" xr:uid="{B25F1A9F-03AE-4789-8CD2-CB2B419E75D3}"/>
     <hyperlink ref="G27" r:id="rId68" xr:uid="{B387B890-5D29-4BC8-BD6D-1650235DB8E8}"/>
     <hyperlink ref="G34" r:id="rId69" xr:uid="{02D918AE-3B28-49F3-A4B2-B6C4B9C01DDF}"/>
-    <hyperlink ref="I35" r:id="rId70" xr:uid="{A25EED2C-E3BE-4936-92BA-9EBAF31D5CFE}"/>
+    <hyperlink ref="K35" r:id="rId70" xr:uid="{A25EED2C-E3BE-4936-92BA-9EBAF31D5CFE}"/>
     <hyperlink ref="G36" r:id="rId71" xr:uid="{98896767-68B3-4DB5-8485-3E78636914E9}"/>
     <hyperlink ref="G37" r:id="rId72" xr:uid="{A3F78D9B-D934-43E4-B856-3A301E31C3C1}"/>
     <hyperlink ref="G38" r:id="rId73" xr:uid="{C5F561F3-130D-4416-936C-457F8B57B35B}"/>
-    <hyperlink ref="I38" r:id="rId74" xr:uid="{EBE5F2A1-3363-4E43-8C95-B8A920988863}"/>
+    <hyperlink ref="K38" r:id="rId74" xr:uid="{EBE5F2A1-3363-4E43-8C95-B8A920988863}"/>
     <hyperlink ref="G39" r:id="rId75" xr:uid="{6A6D114E-E864-457B-AB2F-99E0D8B52F13}"/>
     <hyperlink ref="G40" r:id="rId76" xr:uid="{39923938-2046-4238-9929-6A2FCC4EF61F}"/>
     <hyperlink ref="G41" r:id="rId77" xr:uid="{0F235A0B-7A89-4D43-B74C-ABF6411EB002}"/>
-    <hyperlink ref="I41" r:id="rId78" xr:uid="{0D89B8C6-BD1A-449E-825E-53B59B06B44D}"/>
-    <hyperlink ref="I42" r:id="rId79" xr:uid="{87AF6788-0691-4D4F-9ECB-AC587B84DBE6}"/>
-    <hyperlink ref="H45" r:id="rId80" xr:uid="{D59AAD8F-2849-4596-A946-37E273530F60}"/>
-    <hyperlink ref="H46" r:id="rId81" xr:uid="{F2EA398D-24CA-477C-85E2-3BF00C359038}"/>
-    <hyperlink ref="H48" r:id="rId82" xr:uid="{D5477E06-23F9-4C66-865A-52CB807308B0}"/>
+    <hyperlink ref="K41" r:id="rId78" xr:uid="{0D89B8C6-BD1A-449E-825E-53B59B06B44D}"/>
+    <hyperlink ref="K42" r:id="rId79" xr:uid="{87AF6788-0691-4D4F-9ECB-AC587B84DBE6}"/>
+    <hyperlink ref="I45" r:id="rId80" xr:uid="{D59AAD8F-2849-4596-A946-37E273530F60}"/>
+    <hyperlink ref="I46" r:id="rId81" xr:uid="{F2EA398D-24CA-477C-85E2-3BF00C359038}"/>
+    <hyperlink ref="I48" r:id="rId82" xr:uid="{D5477E06-23F9-4C66-865A-52CB807308B0}"/>
     <hyperlink ref="G51" r:id="rId83" xr:uid="{344F7BEC-C543-4DA6-A52B-282D37160D95}"/>
-    <hyperlink ref="I52" r:id="rId84" xr:uid="{F599E887-1AAA-4AFD-82B0-AA3A4CD19FEB}"/>
+    <hyperlink ref="K52" r:id="rId84" xr:uid="{F599E887-1AAA-4AFD-82B0-AA3A4CD19FEB}"/>
     <hyperlink ref="G53" r:id="rId85" xr:uid="{73A3D12F-2027-4EB0-8A30-892D3CBCBA51}"/>
-    <hyperlink ref="H55" r:id="rId86" xr:uid="{3FF88A0B-992E-48F5-8F4B-510EB98A96C0}"/>
-    <hyperlink ref="I55" r:id="rId87" xr:uid="{743D22AD-10B9-4FB7-B53F-5EBDFA775042}"/>
-    <hyperlink ref="I58" r:id="rId88" xr:uid="{4BD12333-6288-4684-A8DB-421065625982}"/>
+    <hyperlink ref="I55" r:id="rId86" xr:uid="{3FF88A0B-992E-48F5-8F4B-510EB98A96C0}"/>
+    <hyperlink ref="K55" r:id="rId87" xr:uid="{743D22AD-10B9-4FB7-B53F-5EBDFA775042}"/>
+    <hyperlink ref="K58" r:id="rId88" xr:uid="{4BD12333-6288-4684-A8DB-421065625982}"/>
     <hyperlink ref="G59" r:id="rId89" xr:uid="{39A1C5E3-383D-4003-AC93-2A9194AA589C}"/>
     <hyperlink ref="G60" r:id="rId90" xr:uid="{C103DAA0-30C1-4483-9381-DD31B5B0213F}"/>
-    <hyperlink ref="I61" r:id="rId91" xr:uid="{855C4F7E-271B-46CC-B225-065F91ABBA46}"/>
-    <hyperlink ref="I63" r:id="rId92" xr:uid="{FEA2FAAA-7DEB-414F-B12C-CC5C4D8BAAF4}"/>
+    <hyperlink ref="K61" r:id="rId91" xr:uid="{855C4F7E-271B-46CC-B225-065F91ABBA46}"/>
+    <hyperlink ref="K63" r:id="rId92" xr:uid="{FEA2FAAA-7DEB-414F-B12C-CC5C4D8BAAF4}"/>
     <hyperlink ref="G64" r:id="rId93" xr:uid="{07C4BDCF-FB01-4952-8D5F-C1E304FE2541}"/>
-    <hyperlink ref="I64" r:id="rId94" xr:uid="{8EDD0847-EB81-4059-9034-AD64B511C510}"/>
+    <hyperlink ref="K64" r:id="rId94" xr:uid="{8EDD0847-EB81-4059-9034-AD64B511C510}"/>
     <hyperlink ref="G65" r:id="rId95" xr:uid="{6F4A0415-F987-46E3-8504-102B2744D1CE}"/>
-    <hyperlink ref="I65" r:id="rId96" xr:uid="{47B115A5-B55E-44C2-A5EC-D1111A9A227E}"/>
-    <hyperlink ref="I67" r:id="rId97" xr:uid="{4FE66C51-2B86-4993-A986-52D303FE232B}"/>
-    <hyperlink ref="J68" r:id="rId98" xr:uid="{4AF67FA6-3D24-4F48-80A6-F8EEDB0BF441}"/>
+    <hyperlink ref="K65" r:id="rId96" xr:uid="{47B115A5-B55E-44C2-A5EC-D1111A9A227E}"/>
+    <hyperlink ref="K67" r:id="rId97" xr:uid="{4FE66C51-2B86-4993-A986-52D303FE232B}"/>
+    <hyperlink ref="M68" r:id="rId98" xr:uid="{4AF67FA6-3D24-4F48-80A6-F8EEDB0BF441}"/>
     <hyperlink ref="G72" r:id="rId99" xr:uid="{391EFA0A-4580-49AB-9643-39CF1E0FD273}"/>
-    <hyperlink ref="J71" r:id="rId100" xr:uid="{31E12921-14E3-4231-A3F5-3C3CF28A1F29}"/>
-    <hyperlink ref="I73" r:id="rId101" xr:uid="{50D4E03E-6B6A-465E-87B7-14E280E7E92A}"/>
-    <hyperlink ref="I74" r:id="rId102" xr:uid="{BF9C1A1A-F9F2-4BAA-A71A-D87C143997DD}"/>
-    <hyperlink ref="I75" r:id="rId103" xr:uid="{D904AB63-25C3-4932-99B7-07A10B17E515}"/>
+    <hyperlink ref="M71" r:id="rId100" xr:uid="{31E12921-14E3-4231-A3F5-3C3CF28A1F29}"/>
+    <hyperlink ref="K73" r:id="rId101" xr:uid="{50D4E03E-6B6A-465E-87B7-14E280E7E92A}"/>
+    <hyperlink ref="K74" r:id="rId102" xr:uid="{BF9C1A1A-F9F2-4BAA-A71A-D87C143997DD}"/>
+    <hyperlink ref="K75" r:id="rId103" xr:uid="{D904AB63-25C3-4932-99B7-07A10B17E515}"/>
     <hyperlink ref="G76" r:id="rId104" xr:uid="{5C3FB054-EE1E-4B66-88C6-C755CAC12DA2}"/>
-    <hyperlink ref="I76" r:id="rId105" xr:uid="{2A4FA7B1-9D1B-46BD-8250-F4721FEF6B7C}"/>
+    <hyperlink ref="K76" r:id="rId105" xr:uid="{2A4FA7B1-9D1B-46BD-8250-F4721FEF6B7C}"/>
     <hyperlink ref="G77" r:id="rId106" xr:uid="{8BB7523D-CEE2-4704-8558-17EC75C62330}"/>
-    <hyperlink ref="I78" r:id="rId107" xr:uid="{A6F72A7C-648D-44FF-8703-03FA1ED8ABCD}"/>
-    <hyperlink ref="I79" r:id="rId108" xr:uid="{CFF25C90-4B4F-4B92-89FB-4A708E8FBCBB}"/>
-    <hyperlink ref="I80" r:id="rId109" xr:uid="{D181ACCD-BAB8-4C73-8EE2-BABD5B239842}"/>
+    <hyperlink ref="K78" r:id="rId107" xr:uid="{A6F72A7C-648D-44FF-8703-03FA1ED8ABCD}"/>
+    <hyperlink ref="K79" r:id="rId108" xr:uid="{CFF25C90-4B4F-4B92-89FB-4A708E8FBCBB}"/>
+    <hyperlink ref="K80" r:id="rId109" xr:uid="{D181ACCD-BAB8-4C73-8EE2-BABD5B239842}"/>
     <hyperlink ref="G81" r:id="rId110" xr:uid="{A0A54EFA-7009-484E-BF54-6FC05D1D8CAB}"/>
-    <hyperlink ref="I81" r:id="rId111" xr:uid="{5073F91A-D63B-451F-9206-0E2F31EA5F9E}"/>
+    <hyperlink ref="K81" r:id="rId111" xr:uid="{5073F91A-D63B-451F-9206-0E2F31EA5F9E}"/>
     <hyperlink ref="G82" r:id="rId112" xr:uid="{8611601C-EFE3-48C9-9BD4-D3DA87F835BB}"/>
-    <hyperlink ref="I82" r:id="rId113" xr:uid="{D11E223F-0463-494C-9D9B-045303D1D14B}"/>
-    <hyperlink ref="I83" r:id="rId114" xr:uid="{43172B44-84E7-4716-9D7A-9370B10C0AAD}"/>
-    <hyperlink ref="H84" r:id="rId115" xr:uid="{E34EC7C8-C6E1-4DAF-AD24-E35C265C1C4E}"/>
-    <hyperlink ref="H85" r:id="rId116" xr:uid="{F90D83BF-0F65-4122-A2B0-C6F4D742A3AE}"/>
-    <hyperlink ref="I87" r:id="rId117" xr:uid="{8D5F60AF-1382-4373-9C99-ED336645272B}"/>
+    <hyperlink ref="K82" r:id="rId113" xr:uid="{D11E223F-0463-494C-9D9B-045303D1D14B}"/>
+    <hyperlink ref="K83" r:id="rId114" xr:uid="{43172B44-84E7-4716-9D7A-9370B10C0AAD}"/>
+    <hyperlink ref="I84" r:id="rId115" xr:uid="{E34EC7C8-C6E1-4DAF-AD24-E35C265C1C4E}"/>
+    <hyperlink ref="I85" r:id="rId116" xr:uid="{F90D83BF-0F65-4122-A2B0-C6F4D742A3AE}"/>
+    <hyperlink ref="K87" r:id="rId117" xr:uid="{8D5F60AF-1382-4373-9C99-ED336645272B}"/>
     <hyperlink ref="G90" r:id="rId118" xr:uid="{D0661605-B06E-4AC5-B736-09C3DA4ABE8C}"/>
     <hyperlink ref="G91" r:id="rId119" xr:uid="{4AAC6051-951F-4AB4-B72A-E6D9D0DEF044}"/>
-    <hyperlink ref="H91" r:id="rId120" xr:uid="{6FA1F19D-0882-4AE2-AABF-4F2ACF8F83E2}"/>
-    <hyperlink ref="I91" r:id="rId121" xr:uid="{9EC07AF1-5CF7-483C-B622-746DAB8236CF}"/>
-    <hyperlink ref="J42" r:id="rId122" xr:uid="{E2261B25-9314-4C36-A045-0C1223238B2C}"/>
-    <hyperlink ref="J62" r:id="rId123" xr:uid="{EEA6F03B-4B24-4DD0-ABEC-2755A14E602F}"/>
+    <hyperlink ref="I91" r:id="rId120" xr:uid="{6FA1F19D-0882-4AE2-AABF-4F2ACF8F83E2}"/>
+    <hyperlink ref="K91" r:id="rId121" xr:uid="{9EC07AF1-5CF7-483C-B622-746DAB8236CF}"/>
+    <hyperlink ref="M42" r:id="rId122" xr:uid="{E2261B25-9314-4C36-A045-0C1223238B2C}"/>
+    <hyperlink ref="M62" r:id="rId123" xr:uid="{EEA6F03B-4B24-4DD0-ABEC-2755A14E602F}"/>
     <hyperlink ref="E2" r:id="rId124" display="https://doi.org/10.1504/IJEDPO.2009.028954" xr:uid="{692516D4-CC42-4793-A0D5-3B8ECDFEBBFD}"/>
     <hyperlink ref="E3" r:id="rId125" display="https://doi.org/10.1002/qre.1063" xr:uid="{C3E04136-559C-4C95-A71F-ED3E430FF8F0}"/>
     <hyperlink ref="E4" r:id="rId126" display="https://doi.org/10.1002/qre.1165" xr:uid="{A72FBAB8-5FE5-480E-ADF9-5144510D6182}"/>
@@ -9405,20 +9585,20 @@
     <hyperlink ref="E23" r:id="rId138" display="https://doi.org/10.1002/9781118445112.stat07946" xr:uid="{35A59AA7-19B1-4907-B821-794F8385D5FE}"/>
     <hyperlink ref="E49" r:id="rId139" display="https://www.jasp-online.org/asjournal/summer-2019/designs-of-experiments-doe-in-survivability-testing/" xr:uid="{F359D08E-AE8E-4916-B29B-49D1A002D119}"/>
     <hyperlink ref="E113" r:id="rId140" display="https://doi.org/10.1002/9781119357056.ch18" xr:uid="{933D4C61-B842-46E8-8C85-EF0A66C5F2F1}"/>
-    <hyperlink ref="I115" r:id="rId141" xr:uid="{97900ACB-1389-471A-ADBF-4279F8C6E079}"/>
-    <hyperlink ref="I116" r:id="rId142" xr:uid="{293EFF17-5C8A-43D4-92F4-B936C9A4FFCF}"/>
-    <hyperlink ref="I118" r:id="rId143" xr:uid="{E7FF5511-47A7-44F4-8BAE-76BF462A84B5}"/>
-    <hyperlink ref="I119" r:id="rId144" xr:uid="{E4F6C9F0-EEE5-4957-A4B0-5C6472FBD1E0}"/>
-    <hyperlink ref="I120" r:id="rId145" xr:uid="{CD58E132-90CE-4D9E-8EB0-4994BD4B4DD0}"/>
-    <hyperlink ref="I121" r:id="rId146" xr:uid="{E023AE51-5D3A-4343-B42D-1334FD9C0537}"/>
-    <hyperlink ref="I122" r:id="rId147" xr:uid="{9B603483-4809-4BB3-870B-B9FE8BA25F47}"/>
-    <hyperlink ref="I124" r:id="rId148" xr:uid="{868D39C9-F39F-4DA1-A5B6-80B53DD95CAF}"/>
+    <hyperlink ref="K115" r:id="rId141" xr:uid="{97900ACB-1389-471A-ADBF-4279F8C6E079}"/>
+    <hyperlink ref="K116" r:id="rId142" xr:uid="{293EFF17-5C8A-43D4-92F4-B936C9A4FFCF}"/>
+    <hyperlink ref="K118" r:id="rId143" xr:uid="{E7FF5511-47A7-44F4-8BAE-76BF462A84B5}"/>
+    <hyperlink ref="K119" r:id="rId144" xr:uid="{E4F6C9F0-EEE5-4957-A4B0-5C6472FBD1E0}"/>
+    <hyperlink ref="K120" r:id="rId145" xr:uid="{CD58E132-90CE-4D9E-8EB0-4994BD4B4DD0}"/>
+    <hyperlink ref="K121" r:id="rId146" xr:uid="{E023AE51-5D3A-4343-B42D-1334FD9C0537}"/>
+    <hyperlink ref="K122" r:id="rId147" xr:uid="{9B603483-4809-4BB3-870B-B9FE8BA25F47}"/>
+    <hyperlink ref="K124" r:id="rId148" xr:uid="{868D39C9-F39F-4DA1-A5B6-80B53DD95CAF}"/>
     <hyperlink ref="G125" r:id="rId149" xr:uid="{1A2C7A7A-0B11-4784-A570-D418C79BB6E3}"/>
-    <hyperlink ref="I126" r:id="rId150" xr:uid="{150786E4-33D6-4591-9CE0-7C18E79AD677}"/>
-    <hyperlink ref="I127" r:id="rId151" xr:uid="{4A038D1D-787F-4824-8754-DD691C1591B0}"/>
-    <hyperlink ref="I128" r:id="rId152" xr:uid="{715140CD-EFAD-4585-A4A0-6B2A814345FB}"/>
-    <hyperlink ref="I123" r:id="rId153" xr:uid="{25B3703B-F3C1-4A99-99A5-253F7CF04E55}"/>
-    <hyperlink ref="I117" r:id="rId154" xr:uid="{1410D822-9320-4241-84AA-6547A6022A3B}"/>
+    <hyperlink ref="K126" r:id="rId150" xr:uid="{150786E4-33D6-4591-9CE0-7C18E79AD677}"/>
+    <hyperlink ref="K127" r:id="rId151" xr:uid="{4A038D1D-787F-4824-8754-DD691C1591B0}"/>
+    <hyperlink ref="K128" r:id="rId152" xr:uid="{715140CD-EFAD-4585-A4A0-6B2A814345FB}"/>
+    <hyperlink ref="K123" r:id="rId153" xr:uid="{25B3703B-F3C1-4A99-99A5-253F7CF04E55}"/>
+    <hyperlink ref="K117" r:id="rId154" xr:uid="{1410D822-9320-4241-84AA-6547A6022A3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId155"/>

</xml_diff>

<commit_message>
Add Anna's and Emma's work, remove download button
</commit_message>
<xml_diff>
--- a/test-science-documents-library.xlsx
+++ b/test-science-documents-library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhaman\Documents\test-science-documents-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4069E74B-7678-4BD1-8396-2C33BC0B9AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E04FAB-EB24-4A21-886E-280CB68BA864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="348" windowWidth="30936" windowHeight="17040" tabRatio="212" xr2:uid="{0ADD57B5-79F8-4915-B656-B2883E0E3CC2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="877">
   <si>
     <t>Project</t>
   </si>
@@ -4500,8 +4500,46 @@
     <t>Introduction to Human-Systems Interaction in Operational Test and Evaluation Course</t>
   </si>
   <si>
-    <t xml:space="preserve">
-    Human-System Interaction (HSI) is the study of interfaces between humans and technical systems. The Department of Defense incorporates HSI evaluations into defense acquisition to improve system performance and reduce lifecycle costs. During operational test and evaluation, HSI evaluations characterize how a system’s operational performance is affected by its users. The goal of this course is to provide the theoretical background and practical tools necessary to plan and evaluate HSI test plans, collect and analyze HSI data, and report on HSI results. We will discuss HSI concepts, measurement methods, design of experiments, data analysis, and evaluation and reporting, all from an operational testing perspective. </t>
+    <t>Anna Flowers, John Haman</t>
+  </si>
+  <si>
+    <t>Sequential Space-Filling Designs for Modeling &amp; Simulation Analyses</t>
+  </si>
+  <si>
+    <t>Haman, John T, and Anna Flowers. Sequential Space-Filling Designs for Modeling &amp; Simulation Analyses. IDA Product ID 3003752. Alexandria, VA: Institute for Defense Analyses, 2024.</t>
+  </si>
+  <si>
+    <t>Space-Filling Design, Sequential Space-Filling Design, Adaptive Design, Adaptive Sampling, Modeling and Simulation</t>
+  </si>
+  <si>
+    <t>Emma Mitchell, Rebecca Medlin, John Haman, Keyla Pagan-Rivera, Dhruv Patel</t>
+  </si>
+  <si>
+    <t>A Reliability Assurance Test Planning and Analysis Tool</t>
+  </si>
+  <si>
+    <t>Haman, John T, Rebecca M Medlin, Emma P Mitchell, Keyla Pagán-Rivera, and Dhruv K Patel. A Reliability Assurance Test Planning and Analysis Tool. IDA Product ID 3003359. Institute for Defense Analyses, 2024.</t>
+  </si>
+  <si>
+    <t>Reliability, Assurance Testing, Bayesian, R Shiny, Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human-System Interaction (HSI) is the study of interfaces between humans and technical systems. The Department of Defense incorporates HSI evaluations into defense acquisition to improve system performance and reduce lifecycle costs. During operational test and evaluation, HSI evaluations characterize how a system’s operational performance is affected by its users. The goal of this course is to provide the theoretical background and practical tools necessary to plan and evaluate HSI test plans, collect and analyze HSI data, and report on HSI results. We will discuss HSI concepts, measurement methods, design of experiments, data analysis, and evaluation and reporting, all from an operational testing perspective. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mis.ida.org/app/andrew/Products/d8336190-f4ca-4511-972c-fc61f48fdeef/Materials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mis.ida.org/app/andrew/Products/15e99e6e-1608-4653-a9ce-a417b1b28f58/CoverSheet </t>
+  </si>
+  <si>
+    <t>Miller, Dr Adam M, and Keyla Pagan-Rivera. Introduction to Human-Systems Interaction in Operational Test and Evaluation Course. IDA Product ID 3002009. Alexandria, VA: Institute for Defense Analyses, 2024.</t>
+  </si>
+  <si>
+    <t>Space-filling designs (SFDs) are a rigorous method for designing modeling and simulation (M&amp;S) studies. However, they are hindered by their requirement to choose the final sample size prior to testing. Sequential designs are an alternative that can increase test efficiency by testing small amounts of data at a time. We have conducted a literature review of existing sequential space-filling designs and found the methods most applicable to the test and evaluation (T&amp;E) community.</t>
+  </si>
+  <si>
+    <t>This presentation documents the work of IDA 2024 Summer Associate Emma Mitchell. The work presented details an R Shiny application developed to provide a user-friendly software tool for researchers to use in planning for and analyzing system reliability. Specifically, the presentation details how one can plan for a reliability test using Bayesian Reliability Assurance test methods. Such tests utilize supplementary data and information, including reliability models, prior test results, expert judgment, and knowledge of environmental conditions, to plan for reliability testing, which in turn can often help in reducing the required amount of testing. In the planning phase, the application enables researchers to use Bayesian methods to incorporate supplementary data when determining appropriate test lengths. In the analysis phase, the tool allows researchers to combine information through Bayesian methods, resulting in better uncertainty quantification than traditional methods.</t>
   </si>
 </sst>
 </file>
@@ -4943,11 +4981,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7078B797-123B-4556-84D1-DEC1D433D8DE}">
-  <dimension ref="A1:S129"/>
+  <dimension ref="A1:S131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T129" sqref="T129"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N131" sqref="N131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9415,17 +9453,84 @@
       <c r="D129" s="7" t="s">
         <v>862</v>
       </c>
+      <c r="E129" s="7" t="s">
+        <v>874</v>
+      </c>
       <c r="F129" s="2" t="s">
         <v>620</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>863</v>
+        <v>871</v>
       </c>
       <c r="O129" s="2" t="s">
         <v>582</v>
       </c>
       <c r="P129" s="2" t="s">
         <v>375</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B130" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="E130" s="7" t="s">
+        <v>865</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="N130" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="O130" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="P130" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B131" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>869</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K131" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="N131" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="O131" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="P131" s="2" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -9599,9 +9704,11 @@
     <hyperlink ref="K128" r:id="rId152" xr:uid="{715140CD-EFAD-4585-A4A0-6B2A814345FB}"/>
     <hyperlink ref="K123" r:id="rId153" xr:uid="{25B3703B-F3C1-4A99-99A5-253F7CF04E55}"/>
     <hyperlink ref="K117" r:id="rId154" xr:uid="{1410D822-9320-4241-84AA-6547A6022A3B}"/>
+    <hyperlink ref="K130" r:id="rId155" xr:uid="{BC9B20F0-C55A-4A94-8023-C80F97FD182E}"/>
+    <hyperlink ref="K131" r:id="rId156" xr:uid="{C1B0F285-5295-4705-AC54-4E2D63A5D2AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId155"/>
+  <pageSetup orientation="portrait" r:id="rId157"/>
 </worksheet>
 </file>
 

</xml_diff>